<commit_message>
Working model with some data processing/plotting scripts.
</commit_message>
<xml_diff>
--- a/BuyingJeans.Hw5.xlsx
+++ b/BuyingJeans.Hw5.xlsx
@@ -21,18 +21,18 @@
     <definedName function="false" hidden="false" name="__shared_1_0_5" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_6" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_7" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_11" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_12" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!)))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_18" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$K$42*POWER(ABS(A$15-$B1),$P$42)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_20" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_21" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_22" vbProcedure="false">0.5+0.1*RAND()</definedName>
@@ -45,18 +45,18 @@
     <definedName function="false" hidden="false" name="__shared_2_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!)))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_0" vbProcedure="false">$B$2*((A18*$B18)+(A19*$B19)+(A20*$B20)+(A21*$B21)+(A22*$B22))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_1" vbProcedure="false">(1/$B$2)*#REF!</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_2" vbProcedure="false">1/(1+EXP(($B$5*POWER(A$3/($B$4-A$3),$B$6))+($B$9*POWER(ABS(1-($B$2*A$8)),$B$10))-2))</definedName>
@@ -66,18 +66,18 @@
     <definedName function="false" hidden="false" name="__shared_3_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!)))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44))))))))))))</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -471,7 +471,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
@@ -544,7 +544,6 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="10" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="10" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="11" fontId="0" numFmtId="165" xfId="17">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -634,20 +633,20 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>615960</xdr:colOff>
+      <xdr:colOff>578160</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>131040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>741600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:colOff>699840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -657,7 +656,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9783360" y="131040"/>
-          <a:ext cx="884520" cy="1056960"/>
+          <a:ext cx="884160" cy="1162440"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -678,15 +677,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>527040</xdr:colOff>
+      <xdr:colOff>489240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>115200</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>908280</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:colOff>866520</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -695,8 +694,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9694440" y="469440"/>
-          <a:ext cx="1140120" cy="745560"/>
+          <a:off x="9694440" y="499680"/>
+          <a:ext cx="1139760" cy="820800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -726,15 +725,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>75240</xdr:colOff>
+      <xdr:colOff>33480</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>817560</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:colOff>775440</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -743,8 +742,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10001520" y="390960"/>
-          <a:ext cx="742320" cy="426960"/>
+          <a:off x="10001160" y="421560"/>
+          <a:ext cx="741960" cy="471960"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -765,15 +764,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>279720</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>477360</xdr:colOff>
+      <xdr:colOff>435240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -782,8 +781,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9447120" y="273240"/>
-          <a:ext cx="956520" cy="309600"/>
+          <a:off x="9446760" y="288360"/>
+          <a:ext cx="956160" cy="339480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -816,15 +815,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>591840</xdr:colOff>
+      <xdr:colOff>554040</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>144360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>84240</xdr:colOff>
+      <xdr:colOff>43200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -835,7 +834,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="9759240" y="321480"/>
-          <a:ext cx="251640" cy="186840"/>
+          <a:ext cx="252000" cy="187200"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -854,15 +853,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>123840</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>697320</xdr:colOff>
+      <xdr:colOff>659160</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -871,8 +870,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9291240" y="433440"/>
-          <a:ext cx="573480" cy="635040"/>
+          <a:off x="9291240" y="464040"/>
+          <a:ext cx="573120" cy="695160"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -893,15 +892,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>222480</xdr:colOff>
+      <xdr:colOff>184680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>96120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>202320</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:colOff>160560</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -910,8 +909,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9389880" y="743400"/>
-          <a:ext cx="738720" cy="438480"/>
+          <a:off x="9389880" y="804600"/>
+          <a:ext cx="738360" cy="483480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -941,15 +940,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>609480</xdr:colOff>
+      <xdr:colOff>551520</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>14040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>609840</xdr:colOff>
+      <xdr:colOff>552240</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -960,7 +959,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="14525280" y="4619520"/>
-          <a:ext cx="720" cy="305280"/>
+          <a:ext cx="1080" cy="305640"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -979,15 +978,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>656280</xdr:colOff>
+      <xdr:colOff>618480</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>619200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -998,7 +997,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="9823680" y="549360"/>
-          <a:ext cx="720" cy="305640"/>
+          <a:ext cx="1080" cy="306000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1017,15 +1016,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>519840</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:colOff>485280</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>336960</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:colOff>298800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1034,8 +1033,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8928000" y="5888520"/>
-          <a:ext cx="576360" cy="608760"/>
+          <a:off x="8928000" y="6448320"/>
+          <a:ext cx="576000" cy="653760"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1056,15 +1055,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>564480</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:colOff>529920</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>547920</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:colOff>509760</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1073,8 +1072,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8972640" y="5986080"/>
-          <a:ext cx="742680" cy="442800"/>
+          <a:off x="8972640" y="6546240"/>
+          <a:ext cx="742320" cy="487800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1104,15 +1103,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>657000</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:colOff>625320</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>473400</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:colOff>438480</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>117000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1121,8 +1120,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8305920" y="6472440"/>
-          <a:ext cx="575640" cy="606600"/>
+          <a:off x="8305920" y="7078320"/>
+          <a:ext cx="575280" cy="666720"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1143,15 +1142,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>690480</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:colOff>658800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>506880</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:colOff>471960</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1160,8 +1159,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8339400" y="6568560"/>
-          <a:ext cx="575640" cy="444960"/>
+          <a:off x="8339400" y="7189560"/>
+          <a:ext cx="575280" cy="489960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1200,15 +1199,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>381600</xdr:colOff>
+      <xdr:colOff>347040</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>173520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>604800</xdr:colOff>
+      <xdr:colOff>570600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1219,7 +1218,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="8789760" y="5853240"/>
-          <a:ext cx="223560" cy="229320"/>
+          <a:ext cx="223920" cy="229680"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1238,15 +1237,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>557640</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:colOff>519840</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>374040</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:colOff>332280</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1255,8 +1254,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9725040" y="6292080"/>
-          <a:ext cx="575280" cy="613800"/>
+          <a:off x="9725040" y="6882840"/>
+          <a:ext cx="574920" cy="673920"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1277,15 +1276,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>600840</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:colOff>563040</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>417240</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:colOff>375480</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1294,8 +1293,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9768240" y="6390000"/>
-          <a:ext cx="575280" cy="448200"/>
+          <a:off x="9768240" y="6995880"/>
+          <a:ext cx="574920" cy="493200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1334,15 +1333,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>337680</xdr:colOff>
+      <xdr:colOff>299880</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>26640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>624600</xdr:colOff>
+      <xdr:colOff>587160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1353,7 +1352,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="9505080" y="5163480"/>
-          <a:ext cx="287280" cy="180720"/>
+          <a:ext cx="287640" cy="181080"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1372,15 +1371,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>664200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:colOff>629640</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>480600</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:colOff>442440</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1389,8 +1388,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9072360" y="6743880"/>
-          <a:ext cx="575640" cy="628920"/>
+          <a:off x="9072360" y="7380000"/>
+          <a:ext cx="575280" cy="689040"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1411,15 +1410,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>621720</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:colOff>587160</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>604800</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:colOff>566640</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1428,8 +1427,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9029880" y="6856560"/>
-          <a:ext cx="742320" cy="448200"/>
+          <a:off x="9029880" y="7508160"/>
+          <a:ext cx="741960" cy="478080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1468,15 +1467,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>176400</xdr:colOff>
+      <xdr:colOff>138600</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>35280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>186480</xdr:colOff>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1487,7 +1486,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="9343800" y="5360400"/>
-          <a:ext cx="10440" cy="269280"/>
+          <a:ext cx="10800" cy="269640"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1506,15 +1505,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>191520</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:colOff>156960</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>144720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>271440</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>233280</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1523,8 +1522,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8599680" y="8077320"/>
-          <a:ext cx="839160" cy="1013400"/>
+          <a:off x="8599680" y="8835480"/>
+          <a:ext cx="838800" cy="1103760"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1545,15 +1544,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>129960</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:colOff>95400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>452160</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:colOff>414000</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1562,8 +1561,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8538120" y="8250480"/>
-          <a:ext cx="1081440" cy="714600"/>
+          <a:off x="8538120" y="9024120"/>
+          <a:ext cx="1081080" cy="789840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1593,15 +1592,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>670320</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:colOff>644760</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>649440</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:colOff>620640</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1610,8 +1609,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6800760" y="8157240"/>
-          <a:ext cx="738360" cy="486720"/>
+          <a:off x="6800760" y="8930520"/>
+          <a:ext cx="738000" cy="531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1641,15 +1640,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>469440</xdr:colOff>
+      <xdr:colOff>441000</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>35640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>742320</xdr:colOff>
+      <xdr:colOff>708120</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1660,7 +1659,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="7359120" y="7663680"/>
-          <a:ext cx="1791720" cy="245880"/>
+          <a:ext cx="1792080" cy="246240"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1679,15 +1678,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>670320</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:colOff>644760</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>486000</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1696,8 +1695,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6800760" y="7964280"/>
-          <a:ext cx="574920" cy="688320"/>
+          <a:off x="6800760" y="8706960"/>
+          <a:ext cx="574560" cy="763560"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1715,15 +1714,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>179280</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:colOff>150840</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>160920</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:colOff>128880</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1732,8 +1731,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7068960" y="7594560"/>
-          <a:ext cx="740880" cy="491400"/>
+          <a:off x="7068960" y="8307000"/>
+          <a:ext cx="740520" cy="536400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1775,12 +1774,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.956862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.60392156862745"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -1975,7 +1974,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>1</v>
@@ -2045,7 +2044,7 @@
       </c>
       <c r="C16" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B16)),$B$22))/C$21</f>
-        <v>0.20678240822088</v>
+        <v>0.201022740139605</v>
       </c>
       <c r="D16" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B16)),$B$22))/D$21</f>
@@ -2129,7 +2128,7 @@
       </c>
       <c r="C17" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B17)),$B$22))/C$21</f>
-        <v>0.202330663747127</v>
+        <v>0.205445707256609</v>
       </c>
       <c r="D17" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B17)),$B$22))/D$21</f>
@@ -2213,7 +2212,7 @@
       </c>
       <c r="C18" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B18)),$B$22))/C$21</f>
-        <v>0.197357227227484</v>
+        <v>0.201022740139605</v>
       </c>
       <c r="D18" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B18)),$B$22))/D$21</f>
@@ -2297,7 +2296,7 @@
       </c>
       <c r="C19" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B19)),$B$22))/C$21</f>
-        <v>0.192249488550363</v>
+        <v>0.196081453344151</v>
       </c>
       <c r="D19" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B19)),$B$22))/D$21</f>
@@ -2381,7 +2380,7 @@
       </c>
       <c r="C20" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B20)),$B$22))/C$21</f>
-        <v>0.187104460349839</v>
+        <v>0.191006732558995</v>
       </c>
       <c r="D20" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B20)),$B$22))/D$21</f>
@@ -2467,7 +2466,7 @@
       </c>
       <c r="C21" s="19" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B16)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B17)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B18)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B20)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B21)),$B$22))</f>
-        <v>4.83600132430909</v>
+        <v>4.8674660247389</v>
       </c>
       <c r="D21" s="19" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B16)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B17)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B18)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B20)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B21)),$B$22))</f>
@@ -2598,7 +2597,7 @@
       </c>
       <c r="C24" s="9" t="n">
         <f aca="false">C$15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="9" t="n">
         <f aca="false">D$15</f>
@@ -2630,7 +2629,7 @@
       </c>
       <c r="C25" s="17" t="n">
         <f aca="false">C16*L16*U16/C$30</f>
-        <v>0.116851932076485</v>
+        <v>0.112111561114107</v>
       </c>
       <c r="D25" s="17" t="n">
         <f aca="false">D16*M16*V16/D$30</f>
@@ -2660,7 +2659,7 @@
       </c>
       <c r="C26" s="17" t="n">
         <f aca="false">C17*L17*U17/C$30</f>
-        <v>0.191493283013598</v>
+        <v>0.191898602762028</v>
       </c>
       <c r="D26" s="17" t="n">
         <f aca="false">D17*M17*V17/D$30</f>
@@ -2690,7 +2689,7 @@
       </c>
       <c r="C27" s="17" t="n">
         <f aca="false">C18*L18*U18/C$30</f>
-        <v>0.277556275524</v>
+        <v>0.279014072125388</v>
       </c>
       <c r="D27" s="17" t="n">
         <f aca="false">D18*M18*V18/D$30</f>
@@ -2720,7 +2719,7 @@
       </c>
       <c r="C28" s="17" t="n">
         <f aca="false">C19*L19*U19/C$30</f>
-        <v>0.25310076221492</v>
+        <v>0.254769643815602</v>
       </c>
       <c r="D28" s="17" t="n">
         <f aca="false">D19*M19*V19/D$30</f>
@@ -2750,7 +2749,7 @@
       </c>
       <c r="C29" s="17" t="n">
         <f aca="false">C20*L20*U20/C$30</f>
-        <v>0.160997747170996</v>
+        <v>0.162206120182875</v>
       </c>
       <c r="D29" s="17" t="n">
         <f aca="false">D20*M20*V20/D$30</f>
@@ -2778,7 +2777,7 @@
       <c r="B30" s="9"/>
       <c r="C30" s="19" t="n">
         <f aca="false">C16*L16*U16+C17*L17*U17+C18*L18*U18+C19*L19*U19+C20*L20*U20</f>
-        <v>0.0402288739155631</v>
+        <v>0.0407619520007554</v>
       </c>
       <c r="D30" s="19" t="n">
         <f aca="false">D16*M16*V16+D17*M17*V17+D18*M18*V18+D19*M19*V19+D20*M20*V20</f>
@@ -2811,7 +2810,7 @@
       </c>
       <c r="C31" s="17" t="n">
         <f aca="false">MAX(C25:C29)</f>
-        <v>0.277556275524</v>
+        <v>0.279014072125388</v>
       </c>
       <c r="D31" s="17" t="n">
         <f aca="false">MAX(D25:D29)</f>
@@ -2881,7 +2880,7 @@
       </c>
       <c r="C34" s="9" t="n">
         <f aca="false">C$15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="9" t="n">
         <f aca="false">D$15</f>
@@ -2928,27 +2927,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(C$15-$B35),$P$42)))/C$40</f>
-        <v>0.412419623481954</v>
+        <v>0.109571793289609</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(D$15-$B35),$P$42)))/D$40</f>
-        <v>0.102492146472971</v>
+        <v>0.112625764569117</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(E$15-$B35),$P$42)))/E$40</f>
-        <v>0.103696075875112</v>
+        <v>0.115753389765256</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(F$15-$B35),$P$42)))/F$40</f>
-        <v>0.00575984883477309</v>
+        <v>0.00503844425050914</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(G$15-$B35),$P$42)))/G$40</f>
-        <v>0.02354414975759</v>
+        <v>0.0209716640205344</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(H$15-$B35),$P$42)))/H$40</f>
-        <v>0.00157316473357589</v>
+        <v>0.0019791413498414</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="23"/>
@@ -2974,27 +2973,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(C$15-$B36),$P$42)))/C$40</f>
-        <v>0.438117191305172</v>
+        <v>0.369994567439969</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(D$15-$B36),$P$42)))/D$40</f>
-        <v>0.366279106906769</v>
+        <v>0.371434885603545</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(E$15-$B36),$P$42)))/E$40</f>
-        <v>0.366949785410572</v>
+        <v>0.372814945879753</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(F$15-$B36),$P$42)))/F$40</f>
-        <v>0.0298058357104573</v>
+        <v>0.027312654741462</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(G$15-$B36),$P$42)))/G$40</f>
-        <v>0.108891370751213</v>
+        <v>0.102656559510512</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(H$15-$B36),$P$42)))/H$40</f>
-        <v>0.00990758491797839</v>
+        <v>0.0115892694543512</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="23"/>
@@ -3019,27 +3018,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(C$15-$B37),$P$42)))/C$40</f>
-        <v>0.120409317924385</v>
+        <v>0.389967275176333</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(D$15-$B37),$P$42)))/D$40</f>
-        <v>0.403297253172548</v>
+        <v>0.384426933535141</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(E$15-$B37),$P$42)))/E$40</f>
-        <v>0.400980236455252</v>
+        <v>0.378875702254634</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(F$15-$B37),$P$42)))/F$40</f>
-        <v>0.129468712762877</v>
+        <v>0.123902916698189</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(G$15-$B37),$P$42)))/G$40</f>
-        <v>0.36926896064457</v>
+        <v>0.366388737282764</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(H$15-$B37),$P$42)))/H$40</f>
-        <v>0.0537021367246609</v>
+        <v>0.0586865563240032</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="23"/>
@@ -3064,27 +3063,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(C$15-$B38),$P$42)))/C$40</f>
-        <v>0.0247626866659662</v>
+        <v>0.1080229721492</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(D$15-$B38),$P$42)))/D$40</f>
-        <v>0.106938212736443</v>
+        <v>0.108443484941986</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(E$15-$B38),$P$42)))/E$40</f>
-        <v>0.107134022869113</v>
+        <v>0.108846404946495</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(F$15-$B38),$P$42)))/F$40</f>
-        <v>0.414917766263975</v>
+        <v>0.412922077059615</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(G$15-$B38),$P$42)))/G$40</f>
-        <v>0.390484393598837</v>
+        <v>0.403012818955326</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(H$15-$B38),$P$42)))/H$40</f>
-        <v>0.236904230336027</v>
+        <v>0.243500791278567</v>
       </c>
       <c r="J38" s="23"/>
       <c r="K38" s="16"/>
@@ -3108,27 +3107,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(C$15-$B39),$P$42)))/C$40</f>
-        <v>0.00429118062252225</v>
+        <v>0.0224433919448887</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(D$15-$B39),$P$42)))/D$40</f>
-        <v>0.0209932807112684</v>
+        <v>0.0230689313502107</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(E$15-$B39),$P$42)))/E$40</f>
-        <v>0.021239879389952</v>
+        <v>0.0237095571538618</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(F$15-$B39),$P$42)))/F$40</f>
-        <v>0.420047836427918</v>
+        <v>0.430823907250224</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(G$15-$B39),$P$42)))/G$40</f>
-        <v>0.10781112524779</v>
+        <v>0.106970220230864</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(H$15-$B39),$P$42)))/H$40</f>
-        <v>0.697912883287758</v>
+        <v>0.684244241593237</v>
       </c>
       <c r="J39" s="23"/>
       <c r="K39" s="16"/>
@@ -3155,27 +3154,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(C$15-$B35),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(C$15-$B36),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(C$15-$B37),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(C$15-$B38),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(C$15-$B39),$P$42)))</f>
-        <v>1.38440278480228</v>
+        <v>1.55533732782674</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(D$15-$B35),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(D$15-$B36),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(D$15-$B37),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(D$15-$B38),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(D$15-$B39),$P$42)))</f>
-        <v>1.50392955801545</v>
+        <v>1.57775277120949</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(E$15-$B35),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(E$15-$B36),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(E$15-$B37),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(E$15-$B38),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(E$15-$B39),$P$42)))</f>
-        <v>1.51261983651486</v>
+        <v>1.60086977365732</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(F$15-$B35),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(F$15-$B36),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(F$15-$B37),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(F$15-$B38),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(F$15-$B39),$P$42)))</f>
-        <v>1.44395615716192</v>
+        <v>1.40783890936758</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(G$15-$B35),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(G$15-$B36),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(G$15-$B37),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(G$15-$B38),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(G$15-$B39),$P$42)))</f>
-        <v>1.55327759484224</v>
+        <v>1.50499098585712</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(H$15-$B35),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(H$15-$B36),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(H$15-$B37),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(H$15-$B38),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(H$15-$B39),$P$42)))</f>
-        <v>1.43284358828448</v>
+        <v>1.4614664460625</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -3205,27 +3204,27 @@
       </c>
       <c r="C41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.56044510002248</v>
+        <v>0.55257450286299</v>
       </c>
       <c r="D41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.59627826102078</v>
+        <v>0.534380166558549</v>
       </c>
       <c r="E41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.58868712624535</v>
+        <v>0.516126016015187</v>
       </c>
       <c r="F41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.512288254033774</v>
+        <v>0.542440538993105</v>
       </c>
       <c r="G41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.555862734140828</v>
+        <v>0.595273476792499</v>
       </c>
       <c r="H41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.580438317870721</v>
+        <v>0.533194740116596</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -3355,27 +3354,27 @@
       </c>
       <c r="C44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.576098961522803</v>
+        <v>0.528929903218523</v>
       </c>
       <c r="D44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.542094729514793</v>
+        <v>0.510010966006666</v>
       </c>
       <c r="E44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.520724000036716</v>
+        <v>0.55677794078365</v>
       </c>
       <c r="F44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.588970260042697</v>
+        <v>0.531609748257324</v>
       </c>
       <c r="G44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.513187851104885</v>
+        <v>0.596812033560127</v>
       </c>
       <c r="H44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.545291320327669</v>
+        <v>0.507642987929285</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
@@ -3409,27 +3408,27 @@
       </c>
       <c r="C45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.550858240341768</v>
+        <v>0.546469406131655</v>
       </c>
       <c r="D45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.567236266331747</v>
+        <v>0.551273025013506</v>
       </c>
       <c r="E45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.550546992337331</v>
+        <v>0.579985120613128</v>
       </c>
       <c r="F45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.539802527753636</v>
+        <v>0.526010338449851</v>
       </c>
       <c r="G45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.568287963233888</v>
+        <v>0.534682932402939</v>
       </c>
       <c r="H45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.503864612150937</v>
+        <v>0.555201384425163</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -3579,12 +3578,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.956862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.60392156862745"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -3685,7 +3684,7 @@
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">$B$2*((C25*$B25)+(C26*$B26)+(C27*$B27)+(C28*$B28)+(C29*$B29))</f>
-        <v>0.450702482617565</v>
+        <v>0.486782278028391</v>
       </c>
       <c r="D8" s="9" t="n">
         <f aca="false">$B$2*((D25*$B25)+(D26*$B26)+(D27*$B27)+(D28*$B28)+(D29*$B29))</f>
@@ -3717,7 +3716,7 @@
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">(1/$B$2)*C8</f>
-        <v>1.80280993047026</v>
+        <v>1.94712911211356</v>
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">(1/$B$2)*D8</f>
@@ -3760,7 +3759,7 @@
       </c>
       <c r="C12" s="17" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(C$3/($B$4-C$3),$B$6))+($B$9*POWER(ABS(1-($B$2*C$8)),$B$10))-2))</f>
-        <v>0.653028146846345</v>
+        <v>0.658420962444354</v>
       </c>
       <c r="D12" s="17" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(D$3/($B$4-D$3),$B$6))+($B$9*POWER(ABS(1-($B$2*D$8)),$B$10))-2))</f>
@@ -3788,7 +3787,7 @@
       <c r="B13" s="16"/>
       <c r="C13" s="14" t="n">
         <f aca="false">($B$5*POWER(C$3/($B$4-C$3),$B$6))+($B$9*POWER(ABS(1-(C$8)),$B$10))-2</f>
-        <v>-1.36080175778888</v>
+        <v>-1.41830475647405</v>
       </c>
       <c r="D13" s="14" t="n">
         <f aca="false">($B$5*POWER(D$3/($B$4-D$3),$B$6))+($B$9*POWER(ABS(1-(D$8)),$B$10))-2</f>
@@ -3814,27 +3813,27 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
       <c r="A14" s="14"/>
       <c r="B14" s="16"/>
-      <c r="C14" s="30" t="n">
+      <c r="C14" s="0" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(C$3/($B$4-C$3),$B$6))+($B$9*POWER(ABS(1-(C$8)),$B$10))-2))</f>
-        <v>0.795889973464663</v>
-      </c>
-      <c r="D14" s="30" t="n">
+        <v>0.805072518134626</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(D$3/($B$4-D$3),$B$6))+($B$9*POWER(ABS(1-(D$8)),$B$10))-2))</f>
         <v>0.797892771404972</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="0" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(E$3/($B$4-E$3),$B$6))+($B$9*POWER(ABS(1-(E$8)),$B$10))-2))</f>
         <v>0.807586745046819</v>
       </c>
-      <c r="F14" s="30" t="n">
+      <c r="F14" s="0" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(F$3/($B$4-F$3),$B$6))+($B$9*POWER(ABS(1-(F$8)),$B$10))-2))</f>
         <v>0.834686215143725</v>
       </c>
-      <c r="G14" s="30" t="n">
+      <c r="G14" s="0" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(G$3/($B$4-G$3),$B$6))+($B$9*POWER(ABS(1-(G$8)),$B$10))-2))</f>
         <v>0.827051861360183</v>
       </c>
-      <c r="H14" s="30" t="n">
+      <c r="H14" s="0" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(H$3/($B$4-H$3),$B$6))+($B$9*POWER(ABS(1-(H$8)),$B$10))-2))</f>
         <v>0.842334531957283</v>
       </c>
@@ -3845,7 +3844,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="29" t="n">
         <v>1</v>
@@ -3865,44 +3864,44 @@
       <c r="K15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="31" t="n">
+      <c r="L15" s="30" t="n">
         <v>0.6</v>
       </c>
-      <c r="M15" s="31" t="n">
+      <c r="M15" s="30" t="n">
         <v>0.7</v>
       </c>
-      <c r="N15" s="31" t="n">
+      <c r="N15" s="30" t="n">
         <v>0.5</v>
       </c>
-      <c r="O15" s="31" t="n">
+      <c r="O15" s="30" t="n">
         <v>0.7</v>
       </c>
-      <c r="P15" s="31" t="n">
+      <c r="P15" s="30" t="n">
         <v>0.9</v>
       </c>
-      <c r="Q15" s="31" t="n">
+      <c r="Q15" s="30" t="n">
         <v>0.9</v>
       </c>
       <c r="R15" s="13"/>
       <c r="T15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U15" s="31" t="n">
+      <c r="U15" s="30" t="n">
         <v>0.6</v>
       </c>
-      <c r="V15" s="31" t="n">
+      <c r="V15" s="30" t="n">
         <v>0.4</v>
       </c>
-      <c r="W15" s="31" t="n">
+      <c r="W15" s="30" t="n">
         <v>0.8</v>
       </c>
-      <c r="X15" s="31" t="n">
+      <c r="X15" s="30" t="n">
         <v>0.8</v>
       </c>
-      <c r="Y15" s="31" t="n">
+      <c r="Y15" s="30" t="n">
         <v>0.7</v>
       </c>
-      <c r="Z15" s="31" t="n">
+      <c r="Z15" s="30" t="n">
         <v>0.9</v>
       </c>
     </row>
@@ -3915,7 +3914,7 @@
       </c>
       <c r="C16" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B16)),$B$22))/C$21</f>
-        <v>0.277477450256606</v>
+        <v>0.196613826922696</v>
       </c>
       <c r="D16" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B16)),$B$22))/D$21</f>
@@ -3999,7 +3998,7 @@
       </c>
       <c r="C17" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B17)),$B$22))/C$21</f>
-        <v>0.223207543889507</v>
+        <v>0.244417829384431</v>
       </c>
       <c r="D17" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B17)),$B$22))/D$21</f>
@@ -4083,7 +4082,7 @@
       </c>
       <c r="C18" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B18)),$B$22))/C$21</f>
-        <v>0.174029212626305</v>
+        <v>0.196613826922696</v>
       </c>
       <c r="D18" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B18)),$B$22))/D$21</f>
@@ -4167,7 +4166,7 @@
       </c>
       <c r="C19" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B19)),$B$22))/C$21</f>
-        <v>0.133888642207178</v>
+        <v>0.153294771738268</v>
       </c>
       <c r="D19" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B19)),$B$22))/D$21</f>
@@ -4251,7 +4250,7 @@
       </c>
       <c r="C20" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B20)),$B$22))/C$21</f>
-        <v>0.102078249338077</v>
+        <v>0.117936687385746</v>
       </c>
       <c r="D20" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B20)),$B$22))/D$21</f>
@@ -4337,7 +4336,7 @@
       </c>
       <c r="C21" s="19" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B16)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B17)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B18)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B20)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B21)),$B$22))</f>
-        <v>3.60389645744265</v>
+        <v>4.09135455673799</v>
       </c>
       <c r="D21" s="19" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B16)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B17)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B18)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B20)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B21)),$B$22))</f>
@@ -4468,7 +4467,7 @@
       </c>
       <c r="C24" s="9" t="n">
         <f aca="false">C$15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="9" t="n">
         <f aca="false">D$15</f>
@@ -4500,7 +4499,7 @@
       </c>
       <c r="C25" s="17" t="n">
         <f aca="false">C16*L16*U16/C$30</f>
-        <v>0.178812410509045</v>
+        <v>0.120473796665108</v>
       </c>
       <c r="D25" s="17" t="n">
         <f aca="false">D16*M16*V16/D$30</f>
@@ -4530,7 +4529,7 @@
       </c>
       <c r="C26" s="17" t="n">
         <f aca="false">C17*L17*U17/C$30</f>
-        <v>0.24090641303894</v>
+        <v>0.250830852105264</v>
       </c>
       <c r="D26" s="17" t="n">
         <f aca="false">D17*M17*V17/D$30</f>
@@ -4560,7 +4559,7 @@
       </c>
       <c r="C27" s="17" t="n">
         <f aca="false">C18*L18*U18/C$30</f>
-        <v>0.279105134200422</v>
+        <v>0.299825319154423</v>
       </c>
       <c r="D27" s="17" t="n">
         <f aca="false">D18*M18*V18/D$30</f>
@@ -4591,7 +4590,7 @@
       </c>
       <c r="C28" s="17" t="n">
         <f aca="false">C19*L19*U19/C$30</f>
-        <v>0.201010919975895</v>
+        <v>0.218832506601364</v>
       </c>
       <c r="D28" s="17" t="n">
         <f aca="false">D19*M19*V19/D$30</f>
@@ -4613,7 +4612,7 @@
         <f aca="false">H19*Q19*Z19/H$30</f>
         <v>0.316250711282517</v>
       </c>
-      <c r="J28" s="30" t="n">
+      <c r="J28" s="0" t="n">
         <f aca="false">IF(C28=C$31,B28,0)</f>
         <v>0</v>
       </c>
@@ -4625,7 +4624,7 @@
       </c>
       <c r="C29" s="17" t="n">
         <f aca="false">C20*L20*U20/C$30</f>
-        <v>0.100165122275698</v>
+        <v>0.110037525473841</v>
       </c>
       <c r="D29" s="17" t="n">
         <f aca="false">D20*M20*V20/D$30</f>
@@ -4653,7 +4652,7 @@
       <c r="B30" s="9"/>
       <c r="C30" s="19" t="n">
         <f aca="false">C16*L16*U16+C17*L17*U17+C18*L18*U18+C19*L19*U19+C20*L20*U20</f>
-        <v>0.0352768844061178</v>
+        <v>0.0371006607262591</v>
       </c>
       <c r="D30" s="19" t="n">
         <f aca="false">D16*M16*V16+D17*M17*V17+D18*M18*V18+D19*M19*V19+D20*M20*V20</f>
@@ -4686,7 +4685,7 @@
       </c>
       <c r="C31" s="17" t="n">
         <f aca="false">MAX(C25:C29)</f>
-        <v>0.279105134200422</v>
+        <v>0.299825319154423</v>
       </c>
       <c r="D31" s="17" t="n">
         <f aca="false">MAX(D25:D29)</f>
@@ -4745,7 +4744,7 @@
       </c>
       <c r="C34" s="9" t="n">
         <f aca="false">C$15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="9" t="n">
         <f aca="false">D$15</f>
@@ -4777,27 +4776,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))/C$40</f>
-        <v>0.266355887165445</v>
+        <v>0.111096974456764</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))/D$40</f>
-        <v>0.109313911311911</v>
+        <v>0.115627503964838</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))/E$40</f>
-        <v>0.112773996781592</v>
+        <v>0.105817621720226</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))/F$40</f>
-        <v>0.01440929356139</v>
+        <v>0.0186027474855184</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))/G$40</f>
-        <v>0.0466391041332201</v>
+        <v>0.0370382092430307</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))/H$40</f>
-        <v>0.0125681871136524</v>
+        <v>0.0157081370616058</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -4809,27 +4808,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))/C$40</f>
-        <v>0.43579768632894</v>
+        <v>0.246930460626575</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))/D$40</f>
-        <v>0.246522374988936</v>
+        <v>0.247859639449196</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))/E$40</f>
-        <v>0.2472921447679</v>
+        <v>0.245649473740705</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))/F$40</f>
-        <v>0.0455941903025362</v>
+        <v>0.053814442841885</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))/G$40</f>
-        <v>0.118002958968739</v>
+        <v>0.105156756055228</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))/H$40</f>
-        <v>0.0397105252959438</v>
+        <v>0.0459734551555964</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -4840,27 +4839,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))/C$40</f>
-        <v>0.200736002378251</v>
+        <v>0.38285230338765</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))/D$40</f>
-        <v>0.386523007963855</v>
+        <v>0.373714414732407</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))/E$40</f>
-        <v>0.379438711669599</v>
+        <v>0.393848160633783</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))/F$40</f>
-        <v>0.128733728863626</v>
+        <v>0.139730272828152</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))/G$40</f>
-        <v>0.255293206517965</v>
+        <v>0.252393704093618</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))/H$40</f>
-        <v>0.113453824201154</v>
+        <v>0.122278632020845</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -4871,27 +4870,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))/C$40</f>
-        <v>0.07345786149312</v>
+        <v>0.186096256625295</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))/D$40</f>
-        <v>0.18578870765238</v>
+        <v>0.186796521388851</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))/E$40</f>
-        <v>0.186368835652648</v>
+        <v>0.185130855825242</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))/F$40</f>
-        <v>0.307444781085347</v>
+        <v>0.309437738567803</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))/G$40</f>
-        <v>0.387665988020346</v>
+        <v>0.415197764374003</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))/H$40</f>
-        <v>0.283393766353744</v>
+        <v>0.286368043738465</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -4900,27 +4899,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))/C$40</f>
-        <v>0.0236525626342437</v>
+        <v>0.073024004903716</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))/D$40</f>
-        <v>0.071851998082918</v>
+        <v>0.0760019204647085</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))/E$40</f>
-        <v>0.0741263111282615</v>
+        <v>0.0695538880800444</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))/F$40</f>
-        <v>0.503818006187101</v>
+        <v>0.478414798276642</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))/G$40</f>
-        <v>0.192398742359729</v>
+        <v>0.19021356623412</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))/H$40</f>
-        <v>0.550873697035506</v>
+        <v>0.529671732023488</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
@@ -4932,27 +4931,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))</f>
-        <v>2.07627861831508</v>
+        <v>2.36341119024112</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))</f>
-        <v>2.34096651271164</v>
+        <v>2.42120020626942</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))</f>
-        <v>2.38467344055252</v>
+        <v>2.29742705051583</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))</f>
-        <v>1.79596085674622</v>
+        <v>1.89132405873603</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))</f>
-        <v>2.33406449365496</v>
+        <v>2.17929260626003</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))</f>
-        <v>1.8152981443504</v>
+        <v>1.88796180641873</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -4967,27 +4966,27 @@
       </c>
       <c r="C41" s="29" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.570948166362941</v>
+        <v>0.568774982970208</v>
       </c>
       <c r="D41" s="29" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.60865280685015</v>
+        <v>0.545877281231806</v>
       </c>
       <c r="E41" s="29" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.607462161593139</v>
+        <v>0.530437041847035</v>
       </c>
       <c r="F41" s="29" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.51313583063893</v>
+        <v>0.545747621264309</v>
       </c>
       <c r="G41" s="29" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.569610959235579</v>
+        <v>0.602374689383432</v>
       </c>
       <c r="H41" s="29" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.583612291701138</v>
+        <v>0.535374436778948</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -5023,27 +5022,27 @@
       </c>
       <c r="C42" s="29" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.0132087489962578</v>
+        <v>0.00246774267405272</v>
       </c>
       <c r="D42" s="29" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0083734183292836</v>
+        <v>0.0176161131635308</v>
       </c>
       <c r="E42" s="29" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.011246563186869</v>
+        <v>0.00905572997406125</v>
       </c>
       <c r="F42" s="29" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.00180607559159398</v>
+        <v>0.0056929458770901</v>
       </c>
       <c r="G42" s="29" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.0043849175516516</v>
+        <v>0.00610422096215189</v>
       </c>
       <c r="H42" s="29" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.0169631593674421</v>
+        <v>0.00811042533256114</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
@@ -5085,27 +5084,27 @@
       </c>
       <c r="C43" s="29" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.0180518913175911</v>
+        <v>0.0123318939004093</v>
       </c>
       <c r="D43" s="29" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.012028823196888</v>
+        <v>0.0118902016058564</v>
       </c>
       <c r="E43" s="29" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.00436183551326394</v>
+        <v>0.0101126185432076</v>
       </c>
       <c r="F43" s="29" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.00274339857511222</v>
+        <v>0.0036874820664525</v>
       </c>
       <c r="G43" s="29" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0166325680632144</v>
+        <v>0.0182121512666345</v>
       </c>
       <c r="H43" s="29" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.00337398217990994</v>
+        <v>0.00947502525523305</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
@@ -5145,27 +5144,27 @@
       </c>
       <c r="C44" s="29" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.592344777239487</v>
+        <v>0.538542522899806</v>
       </c>
       <c r="D44" s="29" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.549738635160029</v>
+        <v>0.510629292773083</v>
       </c>
       <c r="E44" s="29" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.528122676173225</v>
+        <v>0.572059839619324</v>
       </c>
       <c r="F44" s="29" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.59391960660927</v>
+        <v>0.535721230916679</v>
       </c>
       <c r="G44" s="29" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.517731399163604</v>
+        <v>0.597764761187136</v>
       </c>
       <c r="H44" s="29" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.564668226810172</v>
+        <v>0.514979591378942</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
@@ -5205,27 +5204,27 @@
       </c>
       <c r="C45" s="29" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.564104705266654</v>
+        <v>0.551685485783964</v>
       </c>
       <c r="D45" s="29" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.576243380233645</v>
+        <v>0.558779057506472</v>
       </c>
       <c r="E45" s="29" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.552696009874344</v>
+        <v>0.599714750871062</v>
       </c>
       <c r="F45" s="29" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.54861060990952</v>
+        <v>0.527223442224786</v>
       </c>
       <c r="G45" s="29" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.581291840532795</v>
+        <v>0.547391032585874</v>
       </c>
       <c r="H45" s="29" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.520173135939986</v>
+        <v>0.561867601163685</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -5239,27 +5238,27 @@
       </c>
       <c r="C46" s="29" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.00201683116145432</v>
+        <v>0.0122533806599677</v>
       </c>
       <c r="D46" s="29" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.00137729563750327</v>
+        <v>0.00232071986421943</v>
       </c>
       <c r="E46" s="29" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.00755508697591722</v>
+        <v>0.00728454351425171</v>
       </c>
       <c r="F46" s="29" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.00595087559893727</v>
+        <v>0.00753527950495482</v>
       </c>
       <c r="G46" s="29" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.00212234281003475</v>
+        <v>0.00643220252357423</v>
       </c>
       <c r="H46" s="29" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.00410422901622951</v>
+        <v>0.00823727114126086</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -5269,27 +5268,27 @@
       </c>
       <c r="C47" s="29" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.00400276691652834</v>
+        <v>0.0148718829546124</v>
       </c>
       <c r="D47" s="29" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.0141511660069227</v>
+        <v>0.00263268264010549</v>
       </c>
       <c r="E47" s="29" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.00846606452949345</v>
+        <v>0.019734385823831</v>
       </c>
       <c r="F47" s="29" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.0128527970518917</v>
+        <v>0.00918290878646076</v>
       </c>
       <c r="G47" s="29" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.0190902188699693</v>
+        <v>0.00593976491130888</v>
       </c>
       <c r="H47" s="29" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.00984802060760558</v>
+        <v>0.00683559841476381</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -5299,27 +5298,27 @@
       </c>
       <c r="C48" s="29" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.00609926197677851</v>
+        <v>0.0113626054581255</v>
       </c>
       <c r="D48" s="29" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.00809733277186751</v>
+        <v>0.0084075075853616</v>
       </c>
       <c r="E48" s="29" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.0119970381446183</v>
+        <v>0.00445171157829464</v>
       </c>
       <c r="F48" s="29" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.017227028068155</v>
+        <v>0.000418335432186723</v>
       </c>
       <c r="G48" s="29" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.00417642413638532</v>
+        <v>0.0141004534624517</v>
       </c>
       <c r="H48" s="29" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.000275910794734955</v>
+        <v>0.0105559325404465</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -5329,27 +5328,27 @@
       </c>
       <c r="C49" s="29" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.0192438592296094</v>
+        <v>0.00852876077406108</v>
       </c>
       <c r="D49" s="29" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.00555371977388859</v>
+        <v>0.00643234736286104</v>
       </c>
       <c r="E49" s="29" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.00783099777065218</v>
+        <v>0.00244613414630294</v>
       </c>
       <c r="F49" s="29" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.0193981288652867</v>
+        <v>0.0186413793172687</v>
       </c>
       <c r="G49" s="29" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.018210006384179</v>
+        <v>0.0101198294293135</v>
       </c>
       <c r="H49" s="29" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.00615912870503962</v>
+        <v>0.000658285412937403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -5359,27 +5358,27 @@
       </c>
       <c r="C50" s="29" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.00340089579112828</v>
+        <v>0.00811640457250178</v>
       </c>
       <c r="D50" s="29" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.0123611723911017</v>
+        <v>0.015335909081623</v>
       </c>
       <c r="E50" s="29" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.0146251932345331</v>
+        <v>0.00816431790590286</v>
       </c>
       <c r="F50" s="29" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.00807258935645223</v>
+        <v>0.00784603483974934</v>
       </c>
       <c r="G50" s="29" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.00814848294481635</v>
+        <v>0.016549012856558</v>
       </c>
       <c r="H50" s="29" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.0156468675006181</v>
+        <v>0.000872418088838458</v>
       </c>
     </row>
   </sheetData>
@@ -5405,12 +5404,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.956862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.60392156862745"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -5449,22 +5448,22 @@
       <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="32" t="n">
+      <c r="C3" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="D3" s="33" t="n">
+      <c r="D3" s="32" t="n">
         <v>12</v>
       </c>
-      <c r="E3" s="33" t="n">
+      <c r="E3" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="33" t="n">
+      <c r="F3" s="32" t="n">
         <v>17</v>
       </c>
-      <c r="G3" s="33" t="n">
+      <c r="G3" s="32" t="n">
         <v>20</v>
       </c>
-      <c r="H3" s="33" t="n">
+      <c r="H3" s="32" t="n">
         <v>25</v>
       </c>
     </row>
@@ -5472,7 +5471,7 @@
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="34" t="n">
+      <c r="B4" s="33" t="n">
         <v>30</v>
       </c>
       <c r="C4" s="13"/>
@@ -5487,7 +5486,7 @@
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="35" t="n">
+      <c r="B5" s="34" t="n">
         <v>0.2</v>
       </c>
       <c r="L5" s="13"/>
@@ -5496,7 +5495,7 @@
       <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="35" t="n">
+      <c r="B6" s="34" t="n">
         <v>1.1</v>
       </c>
     </row>
@@ -5511,7 +5510,7 @@
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">$B$2*((C25*$B25)+(C26*$B26)+(C27*$B27)+(C28*$B28)+(C29*$B29))</f>
-        <v>0.450702482617565</v>
+        <v>0.486782278028391</v>
       </c>
       <c r="D8" s="9" t="n">
         <f aca="false">$B$2*((D25*$B25)+(D26*$B26)+(D27*$B27)+(D28*$B28)+(D29*$B29))</f>
@@ -5538,12 +5537,12 @@
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="35" t="n">
+      <c r="B9" s="34" t="n">
         <v>1.5</v>
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">(1/$B$2)*C8</f>
-        <v>1.80280993047026</v>
+        <v>1.94712911211356</v>
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">(1/$B$2)*D8</f>
@@ -5570,7 +5569,7 @@
       <c r="A10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="35" t="n">
+      <c r="B10" s="34" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5586,7 +5585,7 @@
       </c>
       <c r="C12" s="17" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(C$3/($B$4-C$3),$B$6))+($B$9*POWER(ABS(1-($B$2*C$8)),$B$10))-2))</f>
-        <v>0.673856534703535</v>
+        <v>0.679084712040075</v>
       </c>
       <c r="D12" s="17" t="n">
         <f aca="false">1/(1+EXP(($B$5*POWER(D$3/($B$4-D$3),$B$6))+($B$9*POWER(ABS(1-($B$2*D$8)),$B$10))-2))</f>
@@ -5623,65 +5622,65 @@
       <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="35" t="n">
+      <c r="C15" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="35" t="n">
+      <c r="D15" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="35" t="n">
+      <c r="E15" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="35" t="n">
+      <c r="G15" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="H15" s="35" t="n">
+      <c r="H15" s="34" t="n">
         <v>4</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="36" t="n">
+      <c r="L15" s="35" t="n">
         <v>0.6</v>
       </c>
-      <c r="M15" s="36" t="n">
+      <c r="M15" s="35" t="n">
         <v>0.7</v>
       </c>
-      <c r="N15" s="36" t="n">
+      <c r="N15" s="35" t="n">
         <v>0.5</v>
       </c>
-      <c r="O15" s="36" t="n">
+      <c r="O15" s="35" t="n">
         <v>0.7</v>
       </c>
-      <c r="P15" s="36" t="n">
+      <c r="P15" s="35" t="n">
         <v>0.9</v>
       </c>
-      <c r="Q15" s="36" t="n">
+      <c r="Q15" s="35" t="n">
         <v>0.9</v>
       </c>
       <c r="R15" s="13"/>
       <c r="T15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U15" s="36" t="n">
+      <c r="U15" s="35" t="n">
         <v>0.6</v>
       </c>
-      <c r="V15" s="36" t="n">
+      <c r="V15" s="35" t="n">
         <v>0.4</v>
       </c>
-      <c r="W15" s="36" t="n">
+      <c r="W15" s="35" t="n">
         <v>0.8</v>
       </c>
-      <c r="X15" s="36" t="n">
+      <c r="X15" s="35" t="n">
         <v>0.8</v>
       </c>
-      <c r="Y15" s="36" t="n">
+      <c r="Y15" s="35" t="n">
         <v>0.7</v>
       </c>
-      <c r="Z15" s="36" t="n">
+      <c r="Z15" s="35" t="n">
         <v>0.9</v>
       </c>
     </row>
@@ -5694,7 +5693,7 @@
       </c>
       <c r="C16" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B16)),$B$22))/C$21</f>
-        <v>0.277477450256606</v>
+        <v>0.196613826922696</v>
       </c>
       <c r="D16" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B16)),$B$22))/D$21</f>
@@ -5778,7 +5777,7 @@
       </c>
       <c r="C17" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B17)),$B$22))/C$21</f>
-        <v>0.223207543889507</v>
+        <v>0.244417829384431</v>
       </c>
       <c r="D17" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B17)),$B$22))/D$21</f>
@@ -5862,7 +5861,7 @@
       </c>
       <c r="C18" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B18)),$B$22))/C$21</f>
-        <v>0.174029212626305</v>
+        <v>0.196613826922696</v>
       </c>
       <c r="D18" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B18)),$B$22))/D$21</f>
@@ -5946,7 +5945,7 @@
       </c>
       <c r="C19" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B19)),$B$22))/C$21</f>
-        <v>0.133888642207178</v>
+        <v>0.153294771738268</v>
       </c>
       <c r="D19" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B19)),$B$22))/D$21</f>
@@ -6030,7 +6029,7 @@
       </c>
       <c r="C20" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B20)),$B$22))/C$21</f>
-        <v>0.102078249338077</v>
+        <v>0.117936687385746</v>
       </c>
       <c r="D20" s="17" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B20)),$B$22))/D$21</f>
@@ -6111,12 +6110,12 @@
       <c r="A21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="35" t="n">
+      <c r="B21" s="34" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="19" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(C$15-$B16)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B17)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B18)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B20)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(C$15-$B21)),$B$22))</f>
-        <v>3.60389645744265</v>
+        <v>4.09135455673799</v>
       </c>
       <c r="D21" s="19" t="n">
         <f aca="false">EXP(-$B$21*POWER(ABS($B$2*(D$15-$B16)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B17)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B18)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B20)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(D$15-$B21)),$B$22))</f>
@@ -6144,7 +6143,7 @@
       <c r="J21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="35" t="n">
+      <c r="K21" s="34" t="n">
         <v>1</v>
       </c>
       <c r="L21" s="1" t="n">
@@ -6177,7 +6176,7 @@
       <c r="S21" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="T21" s="35" t="n">
+      <c r="T21" s="34" t="n">
         <v>1</v>
       </c>
       <c r="U21" s="1" t="n">
@@ -6212,7 +6211,7 @@
       <c r="A22" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="35" t="n">
+      <c r="B22" s="34" t="n">
         <v>1.1</v>
       </c>
       <c r="C22" s="13"/>
@@ -6224,14 +6223,14 @@
       <c r="J22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="35" t="n">
+      <c r="K22" s="34" t="n">
         <v>1.5</v>
       </c>
       <c r="L22" s="13"/>
       <c r="S22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="T22" s="35" t="n">
+      <c r="T22" s="34" t="n">
         <v>1.2</v>
       </c>
       <c r="U22" s="13"/>
@@ -6247,7 +6246,7 @@
       </c>
       <c r="C24" s="9" t="n">
         <f aca="false">C$15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="9" t="n">
         <f aca="false">D$15</f>
@@ -6279,7 +6278,7 @@
       </c>
       <c r="C25" s="17" t="n">
         <f aca="false">C16*L16*U16/C$30</f>
-        <v>0.178812410509045</v>
+        <v>0.120473796665108</v>
       </c>
       <c r="D25" s="17" t="n">
         <f aca="false">D16*M16*V16/D$30</f>
@@ -6309,7 +6308,7 @@
       </c>
       <c r="C26" s="17" t="n">
         <f aca="false">C17*L17*U17/C$30</f>
-        <v>0.24090641303894</v>
+        <v>0.250830852105264</v>
       </c>
       <c r="D26" s="17" t="n">
         <f aca="false">D17*M17*V17/D$30</f>
@@ -6339,7 +6338,7 @@
       </c>
       <c r="C27" s="17" t="n">
         <f aca="false">C18*L18*U18/C$30</f>
-        <v>0.279105134200422</v>
+        <v>0.299825319154423</v>
       </c>
       <c r="D27" s="17" t="n">
         <f aca="false">D18*M18*V18/D$30</f>
@@ -6369,7 +6368,7 @@
       </c>
       <c r="C28" s="17" t="n">
         <f aca="false">C19*L19*U19/C$30</f>
-        <v>0.201010919975895</v>
+        <v>0.218832506601364</v>
       </c>
       <c r="D28" s="17" t="n">
         <f aca="false">D19*M19*V19/D$30</f>
@@ -6399,7 +6398,7 @@
       </c>
       <c r="C29" s="17" t="n">
         <f aca="false">C20*L20*U20/C$30</f>
-        <v>0.100165122275698</v>
+        <v>0.110037525473841</v>
       </c>
       <c r="D29" s="17" t="n">
         <f aca="false">D20*M20*V20/D$30</f>
@@ -6427,7 +6426,7 @@
       <c r="B30" s="9"/>
       <c r="C30" s="19" t="n">
         <f aca="false">C16*L16*U16+C17*L17*U17+C18*L18*U18+C19*L19*U19+C20*L20*U20</f>
-        <v>0.0352768844061178</v>
+        <v>0.0371006607262591</v>
       </c>
       <c r="D30" s="19" t="n">
         <f aca="false">D16*M16*V16+D17*M17*V17+D18*M18*V18+D19*M19*V19+D20*M20*V20</f>
@@ -6460,7 +6459,7 @@
       </c>
       <c r="C31" s="17" t="n">
         <f aca="false">MAX(C25:C29)</f>
-        <v>0.279105134200422</v>
+        <v>0.299825319154423</v>
       </c>
       <c r="D31" s="17" t="n">
         <f aca="false">MAX(D25:D29)</f>
@@ -6519,7 +6518,7 @@
       </c>
       <c r="C34" s="9" t="n">
         <f aca="false">C$15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="9" t="n">
         <f aca="false">D$15</f>
@@ -6551,27 +6550,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))/C$40</f>
-        <v>0.256236454431493</v>
+        <v>0.0987041524145507</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))/D$40</f>
-        <v>0.0981730800323153</v>
+        <v>0.105713424360098</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))/E$40</f>
-        <v>0.101741671211566</v>
+        <v>0.102910124683828</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))/F$40</f>
-        <v>0.0166606426031565</v>
+        <v>0.0217464815622469</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))/G$40</f>
-        <v>0.0406632609099584</v>
+        <v>0.0307925619623999</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))/H$40</f>
-        <v>0.0137259297425833</v>
+        <v>0.017999658843852</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -6583,27 +6582,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))/C$40</f>
-        <v>0.420617642623894</v>
+        <v>0.23805450739988</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))/D$40</f>
-        <v>0.237909661213244</v>
+        <v>0.23973146966223</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))/E$40</f>
-        <v>0.238833861412762</v>
+        <v>0.239111921562219</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))/F$40</f>
-        <v>0.047482182794718</v>
+        <v>0.0564244194939039</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))/G$40</f>
-        <v>0.105640278574617</v>
+        <v>0.091700707308299</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))/H$40</f>
-        <v>0.0401779302579051</v>
+        <v>0.0480069940961517</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -6614,27 +6613,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))/C$40</f>
-        <v>0.206798724701163</v>
+        <v>0.393071225669477</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))/D$40</f>
-        <v>0.394283962908036</v>
+        <v>0.377489349165895</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))/E$40</f>
-        <v>0.386223600405754</v>
+        <v>0.383628779101515</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))/F$40</f>
-        <v>0.126564815988499</v>
+        <v>0.137772182140126</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))/G$40</f>
-        <v>0.248958462483168</v>
+        <v>0.244401967487129</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))/H$40</f>
-        <v>0.110049614964763</v>
+        <v>0.120545106167448</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -6645,27 +6644,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))/C$40</f>
-        <v>0.0846481873060752</v>
+        <v>0.192124764795404</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))/D$40</f>
-        <v>0.192007864931407</v>
+        <v>0.193478177439188</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))/E$40</f>
-        <v>0.192753751862495</v>
+        <v>0.192978163663796</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))/F$40</f>
-        <v>0.305254499279639</v>
+        <v>0.307036301196551</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))/G$40</f>
-        <v>0.403813064617499</v>
+        <v>0.435857204135369</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))/H$40</f>
-        <v>0.274424926899489</v>
+        <v>0.27794756150632</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -6674,59 +6673,59 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))/C$40</f>
-        <v>0.0316989909373751</v>
+        <v>0.0780453497206888</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))/D$40</f>
-        <v>0.0776254309149988</v>
+        <v>0.0835875793725893</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))/E$40</f>
-        <v>0.0804471151074232</v>
+        <v>0.0813710109886424</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))/F$40</f>
-        <v>0.504037859333988</v>
+        <v>0.477020615607172</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))/G$40</f>
-        <v>0.200924933414758</v>
+        <v>0.197247559106803</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))/H$40</f>
-        <v>0.56162159813526</v>
+        <v>0.535500679386229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
       <c r="A40" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="35" t="n">
+      <c r="B40" s="34" t="n">
         <v>1.2</v>
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))</f>
-        <v>2.15121128156063</v>
+        <v>2.30196808859475</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))</f>
-        <v>2.29488770317297</v>
+        <v>2.39698794160762</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))</f>
-        <v>2.34278127252029</v>
+        <v>2.35862757782445</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))</f>
-        <v>1.79517748772199</v>
+        <v>1.89685180982009</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))</f>
-        <v>2.24073339205368</v>
+        <v>2.07599509529946</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))</f>
-        <v>1.78055830352728</v>
+        <v>1.86741126294399</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -6739,29 +6738,29 @@
       <c r="B41" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="35" t="n">
+      <c r="C41" s="34" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.597551460471004</v>
-      </c>
-      <c r="D41" s="35" t="n">
+        <v>0.602744834078476</v>
+      </c>
+      <c r="D41" s="34" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.637225579936057</v>
-      </c>
-      <c r="E41" s="35" t="n">
+        <v>0.590427946485579</v>
+      </c>
+      <c r="E41" s="34" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.655790661089122</v>
-      </c>
-      <c r="F41" s="35" t="n">
+        <v>0.577416131645441</v>
+      </c>
+      <c r="F41" s="34" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.544934791559353</v>
-      </c>
-      <c r="G41" s="35" t="n">
+        <v>0.591282799327746</v>
+      </c>
+      <c r="G41" s="34" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.575692196469754</v>
-      </c>
-      <c r="H41" s="35" t="n">
+        <v>0.5972358006984</v>
+      </c>
+      <c r="H41" s="34" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.613650994701311</v>
+        <v>0.624183680303395</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -6795,57 +6794,57 @@
       <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="35" t="n">
+      <c r="C42" s="34" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.0239756284281611</v>
-      </c>
-      <c r="D42" s="35" t="n">
+        <v>0.0830202524084598</v>
+      </c>
+      <c r="D42" s="34" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0938681032974273</v>
-      </c>
-      <c r="E42" s="35" t="n">
+        <v>0.0587753511965275</v>
+      </c>
+      <c r="E42" s="34" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.0180951442103833</v>
-      </c>
-      <c r="F42" s="35" t="n">
+        <v>0.0330264781136066</v>
+      </c>
+      <c r="F42" s="34" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.0995156436692923</v>
-      </c>
-      <c r="G42" s="35" t="n">
+        <v>0.00527881029993296</v>
+      </c>
+      <c r="G42" s="34" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.065895225526765</v>
-      </c>
-      <c r="H42" s="35" t="n">
+        <v>0.0608670283574611</v>
+      </c>
+      <c r="H42" s="34" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.010879655694589</v>
+        <v>0.00352874542586505</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K42" s="35" t="n">
+      <c r="K42" s="34" t="n">
         <f aca="false">agent1!K42</f>
         <v>0.5</v>
       </c>
-      <c r="L42" s="35" t="n">
+      <c r="L42" s="34" t="n">
         <f aca="false">agent1!L42</f>
         <v>0.5</v>
       </c>
-      <c r="M42" s="35" t="n">
+      <c r="M42" s="34" t="n">
         <f aca="false">agent1!M42</f>
         <v>0.1</v>
       </c>
       <c r="O42" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="P42" s="35" t="n">
+      <c r="P42" s="34" t="n">
         <f aca="false">agent1!P42</f>
         <v>1.3</v>
       </c>
-      <c r="Q42" s="35" t="n">
+      <c r="Q42" s="34" t="n">
         <f aca="false">agent1!Q42</f>
         <v>1.1</v>
       </c>
-      <c r="R42" s="35" t="n">
+      <c r="R42" s="34" t="n">
         <f aca="false">agent1!R42</f>
         <v>1.1</v>
       </c>
@@ -6857,57 +6856,57 @@
       <c r="B43" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="35" t="n">
+      <c r="C43" s="34" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.0190402226056904</v>
-      </c>
-      <c r="D43" s="35" t="n">
+        <v>0.0580584730021656</v>
+      </c>
+      <c r="D43" s="34" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.0289808368775994</v>
-      </c>
-      <c r="E43" s="35" t="n">
+        <v>0.00351083222776651</v>
+      </c>
+      <c r="E43" s="34" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.0708039633929729</v>
-      </c>
-      <c r="F43" s="35" t="n">
+        <v>0.0356904822401702</v>
+      </c>
+      <c r="F43" s="34" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.078579015377909</v>
-      </c>
-      <c r="G43" s="35" t="n">
+        <v>0.0702891437336803</v>
+      </c>
+      <c r="G43" s="34" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0123452349100262</v>
-      </c>
-      <c r="H43" s="35" t="n">
+        <v>0.0967177288141102</v>
+      </c>
+      <c r="H43" s="34" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.0270920726004988</v>
+        <v>0.0862896294333041</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K43" s="35" t="n">
+      <c r="K43" s="34" t="n">
         <f aca="false">agent1!K43</f>
         <v>0.1</v>
       </c>
-      <c r="L43" s="35" t="n">
+      <c r="L43" s="34" t="n">
         <f aca="false">agent1!L43</f>
         <v>0.1</v>
       </c>
-      <c r="M43" s="35" t="n">
+      <c r="M43" s="34" t="n">
         <f aca="false">agent1!M43</f>
         <v>0.1</v>
       </c>
       <c r="O43" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="P43" s="35" t="n">
+      <c r="P43" s="34" t="n">
         <f aca="false">agent1!P43</f>
         <v>1.1</v>
       </c>
-      <c r="Q43" s="35" t="n">
+      <c r="Q43" s="34" t="n">
         <f aca="false">agent1!Q43</f>
         <v>1.5</v>
       </c>
-      <c r="R43" s="35" t="n">
+      <c r="R43" s="34" t="n">
         <f aca="false">agent1!R43</f>
         <v>1.1</v>
       </c>
@@ -6917,57 +6916,57 @@
       <c r="B44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="35" t="n">
+      <c r="C44" s="34" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.595623540412635</v>
-      </c>
-      <c r="D44" s="35" t="n">
+        <v>0.60149116110988</v>
+      </c>
+      <c r="D44" s="34" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.605180340865627</v>
-      </c>
-      <c r="E44" s="35" t="n">
+        <v>0.554022933635861</v>
+      </c>
+      <c r="E44" s="34" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.5806483077351</v>
-      </c>
-      <c r="F44" s="35" t="n">
+        <v>0.572743630548939</v>
+      </c>
+      <c r="F44" s="34" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.601505530439317</v>
-      </c>
-      <c r="G44" s="35" t="n">
+        <v>0.54059372371994</v>
+      </c>
+      <c r="G44" s="34" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.583665994321927</v>
-      </c>
-      <c r="H44" s="35" t="n">
+        <v>0.678500398714095</v>
+      </c>
+      <c r="H44" s="34" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.616150576993823</v>
+        <v>0.555769690359011</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K44" s="35" t="n">
+      <c r="K44" s="34" t="n">
         <f aca="false">agent1!K44</f>
         <v>0.3</v>
       </c>
-      <c r="L44" s="35" t="n">
+      <c r="L44" s="34" t="n">
         <f aca="false">agent1!L44</f>
         <v>0.1</v>
       </c>
-      <c r="M44" s="35" t="n">
+      <c r="M44" s="34" t="n">
         <f aca="false">agent1!M44</f>
         <v>0.1</v>
       </c>
       <c r="O44" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="P44" s="35" t="n">
+      <c r="P44" s="34" t="n">
         <f aca="false">agent1!P44</f>
         <v>1.1</v>
       </c>
-      <c r="Q44" s="35" t="n">
+      <c r="Q44" s="34" t="n">
         <f aca="false">agent1!Q44</f>
         <v>1.1</v>
       </c>
-      <c r="R44" s="35" t="n">
+      <c r="R44" s="34" t="n">
         <f aca="false">agent1!R44</f>
         <v>1.1</v>
       </c>
@@ -6977,29 +6976,29 @@
       <c r="B45" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="35" t="n">
+      <c r="C45" s="34" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.566543616214767</v>
-      </c>
-      <c r="D45" s="35" t="n">
+        <v>0.620049976976588</v>
+      </c>
+      <c r="D45" s="34" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.620528820157051</v>
-      </c>
-      <c r="E45" s="35" t="n">
+        <v>0.588572776736692</v>
+      </c>
+      <c r="E45" s="34" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.644742599781603</v>
-      </c>
-      <c r="F45" s="35" t="n">
+        <v>0.642954295454547</v>
+      </c>
+      <c r="F45" s="34" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.562708521867171</v>
-      </c>
-      <c r="G45" s="35" t="n">
+        <v>0.540412498824298</v>
+      </c>
+      <c r="G45" s="34" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.64826154159382</v>
-      </c>
-      <c r="H45" s="35" t="n">
+        <v>0.611212858324871</v>
+      </c>
+      <c r="H45" s="34" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.558886466547847</v>
+        <v>0.600915623595938</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -7011,29 +7010,29 @@
       <c r="B46" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="35" t="n">
+      <c r="C46" s="34" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.046881622588262</v>
-      </c>
-      <c r="D46" s="35" t="n">
+        <v>0.0187642508652061</v>
+      </c>
+      <c r="D46" s="34" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.073841681657359</v>
-      </c>
-      <c r="E46" s="35" t="n">
+        <v>0.0490911838132888</v>
+      </c>
+      <c r="E46" s="34" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.0731169986072928</v>
-      </c>
-      <c r="F46" s="35" t="n">
+        <v>0.0897262067999691</v>
+      </c>
+      <c r="F46" s="34" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.0657479682937264</v>
-      </c>
-      <c r="G46" s="35" t="n">
+        <v>0.0347299406304956</v>
+      </c>
+      <c r="G46" s="34" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.0109307950362563</v>
-      </c>
-      <c r="H46" s="35" t="n">
+        <v>0.0580751593224704</v>
+      </c>
+      <c r="H46" s="34" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.0216247433796525</v>
+        <v>0.0714145719539374</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -7041,29 +7040,29 @@
       <c r="B47" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="35" t="n">
+      <c r="C47" s="34" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.0847881908994168</v>
-      </c>
-      <c r="D47" s="35" t="n">
+        <v>0.0828566430602223</v>
+      </c>
+      <c r="D47" s="34" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.0399116319604218</v>
-      </c>
-      <c r="E47" s="35" t="n">
+        <v>0.00824549053795636</v>
+      </c>
+      <c r="E47" s="34" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.0924287068191916</v>
-      </c>
-      <c r="F47" s="35" t="n">
+        <v>0.0274623518809676</v>
+      </c>
+      <c r="F47" s="34" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.0886631711851805</v>
-      </c>
-      <c r="G47" s="35" t="n">
+        <v>0.0441467586904764</v>
+      </c>
+      <c r="G47" s="34" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.0192317130975425</v>
-      </c>
-      <c r="H47" s="35" t="n">
+        <v>0.0570877508725971</v>
+      </c>
+      <c r="H47" s="34" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.0648675074800849</v>
+        <v>0.0294246757868677</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -7071,29 +7070,29 @@
       <c r="B48" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="35" t="n">
+      <c r="C48" s="34" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.00434854705817997</v>
-      </c>
-      <c r="D48" s="35" t="n">
+        <v>0.035135698877275</v>
+      </c>
+      <c r="D48" s="34" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.0725242669228464</v>
-      </c>
-      <c r="E48" s="35" t="n">
+        <v>0.0401080032810569</v>
+      </c>
+      <c r="E48" s="34" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.0590631149709225</v>
-      </c>
-      <c r="F48" s="35" t="n">
+        <v>0.0882000269833952</v>
+      </c>
+      <c r="F48" s="34" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.0429198287427425</v>
-      </c>
-      <c r="G48" s="35" t="n">
+        <v>0.0681621769908816</v>
+      </c>
+      <c r="G48" s="34" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.0507294083945453</v>
-      </c>
-      <c r="H48" s="35" t="n">
+        <v>0.0453868135809898</v>
+      </c>
+      <c r="H48" s="34" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.0973521770443767</v>
+        <v>0.0490670553874224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -7101,29 +7100,29 @@
       <c r="B49" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="35" t="n">
+      <c r="C49" s="34" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.0898014513310045</v>
-      </c>
-      <c r="D49" s="35" t="n">
+        <v>0.0716909224167466</v>
+      </c>
+      <c r="D49" s="34" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.0245710900519043</v>
-      </c>
-      <c r="E49" s="35" t="n">
+        <v>0.00344528658315539</v>
+      </c>
+      <c r="E49" s="34" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.0704691756982356</v>
-      </c>
-      <c r="F49" s="35" t="n">
+        <v>0.052577887615189</v>
+      </c>
+      <c r="F49" s="34" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.096244278177619</v>
-      </c>
-      <c r="G49" s="35" t="n">
+        <v>0.00738140470348299</v>
+      </c>
+      <c r="G49" s="34" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.05141745894216</v>
-      </c>
-      <c r="H49" s="35" t="n">
+        <v>0.0737344303168356</v>
+      </c>
+      <c r="H49" s="34" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.0816099341027439</v>
+        <v>0.0492956164758653</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -7131,29 +7130,29 @@
       <c r="B50" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="35" t="n">
+      <c r="C50" s="34" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.0810324691236019</v>
-      </c>
-      <c r="D50" s="35" t="n">
+        <v>0.0936710341367871</v>
+      </c>
+      <c r="D50" s="34" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.0913290909025818</v>
-      </c>
-      <c r="E50" s="35" t="n">
+        <v>0.047315001161769</v>
+      </c>
+      <c r="E50" s="34" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.0740386409219355</v>
-      </c>
-      <c r="F50" s="35" t="n">
+        <v>0.0865953681990504</v>
+      </c>
+      <c r="F50" s="34" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.0848824673332274</v>
-      </c>
-      <c r="G50" s="35" t="n">
+        <v>0.0566402089782059</v>
+      </c>
+      <c r="G50" s="34" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.0470003119669855</v>
-      </c>
-      <c r="H50" s="35" t="n">
+        <v>0.0617171615827829</v>
+      </c>
+      <c r="H50" s="34" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.0040224963799119</v>
+        <v>0.0631252941209823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added weak ties to spreadsheet
</commit_message>
<xml_diff>
--- a/BuyingJeans.Hw5.xlsx
+++ b/BuyingJeans.Hw5.xlsx
@@ -21,18 +21,18 @@
     <definedName function="false" hidden="false" name="__shared_1_0_5" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_6" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_7" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_11" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_12" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!)))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_18" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$K$42*POWER(ABS(A$15-$B1),$P$42)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_20" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_21" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_22" vbProcedure="false">0.5+0.1*RAND()</definedName>
@@ -45,18 +45,18 @@
     <definedName function="false" hidden="false" name="__shared_2_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!)))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_0" vbProcedure="false">$B$2*((A18*$B18)+(A19*$B19)+(A20*$B20)+(A21*$B21)+(A22*$B22))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_1" vbProcedure="false">(1/$B$2)*#REF!</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_2" vbProcedure="false">1/(1+EXP(($B$5*POWER(A$3/($B$4-A$3),$B$6))+($B$9*POWER(ABS(1-($B$2*A$8)),$B$10))-2))</definedName>
@@ -66,25 +66,25 @@
     <definedName function="false" hidden="false" name="__shared_3_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!)))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))))))))))))))))</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
   <si>
     <t>Brands</t>
   </si>
@@ -260,6 +260,39 @@
     <t>t=10</t>
   </si>
   <si>
+    <t>weak tie influence</t>
+  </si>
+  <si>
+    <t>weak ties fash</t>
+  </si>
+  <si>
+    <t>beta_ik</t>
+  </si>
+  <si>
+    <t>I=1</t>
+  </si>
+  <si>
+    <t>I=2</t>
+  </si>
+  <si>
+    <t>I=3</t>
+  </si>
+  <si>
+    <t>B_ik</t>
+  </si>
+  <si>
+    <t>#1 grumpy</t>
+  </si>
+  <si>
+    <t>#2 sleepy</t>
+  </si>
+  <si>
+    <t>#3 happy</t>
+  </si>
+  <si>
+    <t>#4 sneezy</t>
+  </si>
+  <si>
     <t>Like-Purchase:   &lt;Like&gt;--&gt;</t>
   </si>
   <si>
@@ -275,7 +308,7 @@
     <numFmt formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)" numFmtId="165"/>
     <numFmt formatCode="0.00" numFmtId="166"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -323,33 +356,6 @@
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00FF0000"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="12">
@@ -633,1153 +639,24 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>578160</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>699840</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9783360" y="131040"/>
-          <a:ext cx="884160" cy="1162440"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>489240</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>145440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>866520</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9694440" y="499680"/>
-          <a:ext cx="1139760" cy="820800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Price &amp; Budget</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>33480</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>775440</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10001160" y="421560"/>
-          <a:ext cx="741960" cy="471960"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7df62a"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>435240</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9446760" y="288360"/>
-          <a:ext cx="956160" cy="339480"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7df62a"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Purchase</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>554040</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>43200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Line 1"/>
-        <xdr:cNvCxnSpPr/>
-        <xdr:nvPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9759240" y="321480"/>
-          <a:ext cx="252000" cy="187200"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28440">
-          <a:solidFill>
-            <a:srgbClr val="1f497d"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>86040</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>659160</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9291240" y="464040"/>
-          <a:ext cx="573120" cy="695160"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>184680</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>160560</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9389880" y="804600"/>
-          <a:ext cx="738360" cy="483480"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Like</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>551520</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>552240</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Line 1"/>
-        <xdr:cNvCxnSpPr/>
-        <xdr:nvPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="14525280" y="4619520"/>
-          <a:ext cx="1080" cy="305640"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28440">
-          <a:solidFill>
-            <a:srgbClr val="1f497d"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>618480</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>619200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Line 1"/>
-        <xdr:cNvCxnSpPr/>
-        <xdr:nvPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9823680" y="549360"/>
-          <a:ext cx="1080" cy="306000"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28440">
-          <a:solidFill>
-            <a:srgbClr val="1f497d"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485280</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>298800</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8928000" y="6448320"/>
-          <a:ext cx="576000" cy="653760"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>529920</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>509760</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8972640" y="6546240"/>
-          <a:ext cx="742320" cy="487800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Like</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>625320</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>438480</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8305920" y="7078320"/>
-          <a:ext cx="575280" cy="666720"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>658800</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>471960</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8339400" y="7189560"/>
-          <a:ext cx="575280" cy="489960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Fash</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>347040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>173520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>570600</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Line 1"/>
-        <xdr:cNvCxnSpPr/>
-        <xdr:nvPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8789760" y="5853240"/>
-          <a:ext cx="223920" cy="229680"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28440">
-          <a:solidFill>
-            <a:srgbClr val="1f497d"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>519840</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>332280</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9725040" y="6882840"/>
-          <a:ext cx="574920" cy="673920"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>563040</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>375480</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9768240" y="6995880"/>
-          <a:ext cx="574920" cy="493200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Fit</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>299880</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>587160</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Line 1"/>
-        <xdr:cNvCxnSpPr/>
-        <xdr:nvPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="9505080" y="5163480"/>
-          <a:ext cx="287640" cy="181080"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28440">
-          <a:solidFill>
-            <a:srgbClr val="1f497d"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>629640</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>442440</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9072360" y="7380000"/>
-          <a:ext cx="575280" cy="689040"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>587160</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>566640</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9029880" y="7508160"/>
-          <a:ext cx="741960" cy="478080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Trust</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>138600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>35280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>149040</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Line 1"/>
-        <xdr:cNvCxnSpPr/>
-        <xdr:nvPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="9343800" y="5360400"/>
-          <a:ext cx="10800" cy="269640"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28440">
-          <a:solidFill>
-            <a:srgbClr val="1f497d"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>156960</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>144720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>233280</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8599680" y="8835480"/>
-          <a:ext cx="838800" cy="1103760"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffff00"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>414000</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8538120" y="9024120"/>
-          <a:ext cx="1081080" cy="789840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Advertise</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>644760</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>620640</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6800760" y="8930520"/>
-          <a:ext cx="738000" cy="531720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Fash</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>441000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>708120</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Line 1"/>
-        <xdr:cNvCxnSpPr/>
-        <xdr:nvPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7359120" y="7663680"/>
-          <a:ext cx="1792080" cy="246240"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38160">
-          <a:solidFill>
-            <a:srgbClr val="ffff00"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>644760</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6800760" y="8706960"/>
-          <a:ext cx="574560" cy="763560"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>150840</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>128880</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7068960" y="8307000"/>
-          <a:ext cx="740520" cy="536400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr bIns="45000" lIns="90000" rIns="90000" tIns="45000"/>
-        <a:p>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Time</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -2927,27 +1804,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(C$15-$B35),$P$42)))/C$40</f>
-        <v>0.109571793289609</v>
+        <v>0.108297176141735</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(D$15-$B35),$P$42)))/D$40</f>
-        <v>0.112625764569117</v>
+        <v>0.116004803771132</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(E$15-$B35),$P$42)))/E$40</f>
-        <v>0.115753389765256</v>
+        <v>0.108717906802216</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(F$15-$B35),$P$42)))/F$40</f>
-        <v>0.00503844425050914</v>
+        <v>0.00565197185505001</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(G$15-$B35),$P$42)))/G$40</f>
-        <v>0.0209716640205344</v>
+        <v>0.0252634565894201</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(H$15-$B35),$P$42)))/H$40</f>
-        <v>0.0019791413498414</v>
+        <v>0.00219664127134893</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="23"/>
@@ -2973,27 +1850,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(C$15-$B36),$P$42)))/C$40</f>
-        <v>0.369994567439969</v>
+        <v>0.369365318897504</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(D$15-$B36),$P$42)))/D$40</f>
-        <v>0.371434885603545</v>
+        <v>0.372921835158266</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(E$15-$B36),$P$42)))/E$40</f>
-        <v>0.372814945879753</v>
+        <v>0.369574889918842</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(F$15-$B36),$P$42)))/F$40</f>
-        <v>0.027312654741462</v>
+        <v>0.0294407474411251</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(G$15-$B36),$P$42)))/G$40</f>
-        <v>0.102656559510512</v>
+        <v>0.11284310510453</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(H$15-$B36),$P$42)))/H$40</f>
-        <v>0.0115892694543512</v>
+        <v>0.0124428905252412</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="23"/>
@@ -3018,27 +1895,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(C$15-$B37),$P$42)))/C$40</f>
-        <v>0.389967275176333</v>
+        <v>0.392315932701291</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(D$15-$B37),$P$42)))/D$40</f>
-        <v>0.384426933535141</v>
+        <v>0.37843469508647</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(E$15-$B37),$P$42)))/E$40</f>
-        <v>0.378875702254634</v>
+        <v>0.391538267528497</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(F$15-$B37),$P$42)))/F$40</f>
-        <v>0.123902916698189</v>
+        <v>0.128671843617798</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(G$15-$B37),$P$42)))/G$40</f>
-        <v>0.366388737282764</v>
+        <v>0.370844965054964</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(H$15-$B37),$P$42)))/H$40</f>
-        <v>0.0586865563240032</v>
+        <v>0.061084660085764</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="23"/>
@@ -3063,27 +1940,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(C$15-$B38),$P$42)))/C$40</f>
-        <v>0.1080229721492</v>
+        <v>0.107839257836182</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(D$15-$B38),$P$42)))/D$40</f>
-        <v>0.108443484941986</v>
+        <v>0.108877612154849</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(E$15-$B38),$P$42)))/E$40</f>
-        <v>0.108846404946495</v>
+        <v>0.107900443828068</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(F$15-$B38),$P$42)))/F$40</f>
-        <v>0.412922077059615</v>
+        <v>0.414655762351118</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(G$15-$B38),$P$42)))/G$40</f>
-        <v>0.403012818955326</v>
+        <v>0.382777220489239</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(H$15-$B38),$P$42)))/H$40</f>
-        <v>0.243500791278567</v>
+        <v>0.246464634505995</v>
       </c>
       <c r="J38" s="23"/>
       <c r="K38" s="16"/>
@@ -3107,27 +1984,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(C$15-$B39),$P$42)))/C$40</f>
-        <v>0.0224433919448887</v>
+        <v>0.0221823144232878</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(D$15-$B39),$P$42)))/D$40</f>
-        <v>0.0230689313502107</v>
+        <v>0.0237610538292827</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(E$15-$B39),$P$42)))/E$40</f>
-        <v>0.0237095571538618</v>
+        <v>0.0222684919223769</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(F$15-$B39),$P$42)))/F$40</f>
-        <v>0.430823907250224</v>
+        <v>0.421579674734909</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(G$15-$B39),$P$42)))/G$40</f>
-        <v>0.106970220230864</v>
+        <v>0.108271252761848</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(H$15-$B39),$P$42)))/H$40</f>
-        <v>0.684244241593237</v>
+        <v>0.67781117361165</v>
       </c>
       <c r="J39" s="23"/>
       <c r="K39" s="16"/>
@@ -3154,27 +2031,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(C$15-$B35),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(C$15-$B36),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(C$15-$B37),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(C$15-$B38),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(C$15-$B39),$P$42)))</f>
-        <v>1.55533732782674</v>
+        <v>1.5460260702041</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(D$15-$B35),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(D$15-$B36),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(D$15-$B37),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(D$15-$B38),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(D$15-$B39),$P$42)))</f>
-        <v>1.57775277120949</v>
+        <v>1.60273534004076</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(E$15-$B35),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(E$15-$B36),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(E$15-$B37),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(E$15-$B38),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(E$15-$B39),$P$42)))</f>
-        <v>1.60086977365732</v>
+        <v>1.54909675506619</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(F$15-$B35),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(F$15-$B36),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(F$15-$B37),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(F$15-$B38),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(F$15-$B39),$P$42)))</f>
-        <v>1.40783890936758</v>
+        <v>1.43870944464774</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(G$15-$B35),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(G$15-$B36),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(G$15-$B37),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(G$15-$B38),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(G$15-$B39),$P$42)))</f>
-        <v>1.50499098585712</v>
+        <v>1.58455265163744</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(H$15-$B35),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(H$15-$B36),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(H$15-$B37),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(H$15-$B38),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(H$15-$B39),$P$42)))</f>
-        <v>1.4614664460625</v>
+        <v>1.47533714245458</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -3204,27 +2081,27 @@
       </c>
       <c r="C41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.55257450286299</v>
+        <v>0.560281287552789</v>
       </c>
       <c r="D41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.534380166558549</v>
+        <v>0.514674681425095</v>
       </c>
       <c r="E41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.516126016015187</v>
+        <v>0.557729857647791</v>
       </c>
       <c r="F41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.542440538993105</v>
+        <v>0.516560098528862</v>
       </c>
       <c r="G41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.595273476792499</v>
+        <v>0.531669058883563</v>
       </c>
       <c r="H41" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.533194740116596</v>
+        <v>0.511650231527165</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -3354,27 +2231,27 @@
       </c>
       <c r="C44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.528929903218523</v>
+        <v>0.512786097778007</v>
       </c>
       <c r="D44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.510010966006666</v>
+        <v>0.50205766283907</v>
       </c>
       <c r="E44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.55677794078365</v>
+        <v>0.510215834248811</v>
       </c>
       <c r="F44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.531609748257324</v>
+        <v>0.549331844318658</v>
       </c>
       <c r="G44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.596812033560127</v>
+        <v>0.516831900319085</v>
       </c>
       <c r="H44" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.507642987929285</v>
+        <v>0.524025741405785</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
@@ -3408,27 +2285,27 @@
       </c>
       <c r="C45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.546469406131655</v>
+        <v>0.544786738837138</v>
       </c>
       <c r="D45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.551273025013506</v>
+        <v>0.50193161140196</v>
       </c>
       <c r="E45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.579985120613128</v>
+        <v>0.50318966396153</v>
       </c>
       <c r="F45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.526010338449851</v>
+        <v>0.588707046210766</v>
       </c>
       <c r="G45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.534682932402939</v>
+        <v>0.555680210608989</v>
       </c>
       <c r="H45" s="15" t="n">
         <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.555201384425163</v>
+        <v>0.553438443923369</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -3553,6 +2430,204 @@
       </c>
       <c r="H50" s="15" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="52">
+      <c r="J52" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="53">
+      <c r="B53" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="L53" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="O53" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="P53" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q53" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="R53" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="54">
+      <c r="B54" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M54" s="15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P54" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="R54" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="55">
+      <c r="B55" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D55" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G55" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="H55" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K55" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="R55" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="56">
+      <c r="B56" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D56" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E56" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F56" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G56" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="H56" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="K56" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L56" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M56" s="15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P56" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="R56" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="57">
+      <c r="B57" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G57" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="H57" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="K57" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L57" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M57" s="15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="P57" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="R57" s="15" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3571,19 +2646,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -3680,7 +2755,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
       <c r="A8" s="14"/>
       <c r="B8" s="9" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">$B$2*((C25*$B25)+(C26*$B26)+(C27*$B27)+(C28*$B28)+(C29*$B29))</f>
@@ -4776,27 +3851,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))/C$40</f>
-        <v>0.111096974456764</v>
+        <v>0.112065937450578</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))/D$40</f>
-        <v>0.115627503964838</v>
+        <v>0.114226448851697</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))/E$40</f>
-        <v>0.105817621720226</v>
+        <v>0.114484155873081</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))/F$40</f>
-        <v>0.0186027474855184</v>
+        <v>0.0165092751236266</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))/G$40</f>
-        <v>0.0370382092430307</v>
+        <v>0.0458684654717235</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))/H$40</f>
-        <v>0.0157081370616058</v>
+        <v>0.0145514355668166</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -4808,27 +3883,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))/C$40</f>
-        <v>0.246930460626575</v>
+        <v>0.247142021389393</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))/D$40</f>
-        <v>0.247859639449196</v>
+        <v>0.247588441214255</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))/E$40</f>
-        <v>0.245649473740705</v>
+        <v>0.247639393681416</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))/F$40</f>
-        <v>0.053814442841885</v>
+        <v>0.0498127716687151</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))/G$40</f>
-        <v>0.105156756055228</v>
+        <v>0.117035220682432</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))/H$40</f>
-        <v>0.0459734551555964</v>
+        <v>0.0437266196936159</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -4839,27 +3914,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))/C$40</f>
-        <v>0.38285230338765</v>
+        <v>0.380875440275599</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))/D$40</f>
-        <v>0.373714414732407</v>
+        <v>0.376511966528432</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))/E$40</f>
-        <v>0.393848160633783</v>
+        <v>0.375995516567611</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))/F$40</f>
-        <v>0.139730272828152</v>
+        <v>0.134531460234398</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))/G$40</f>
-        <v>0.252393704093618</v>
+        <v>0.25512948835354</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))/H$40</f>
-        <v>0.122278632020845</v>
+        <v>0.119205305665062</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -4870,27 +3945,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))/C$40</f>
-        <v>0.186096256625295</v>
+        <v>0.186255696922411</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))/D$40</f>
-        <v>0.186796521388851</v>
+        <v>0.186592136007647</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))/E$40</f>
-        <v>0.185130855825242</v>
+        <v>0.186630535739217</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))/F$40</f>
-        <v>0.309437738567803</v>
+        <v>0.308679456579522</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))/G$40</f>
-        <v>0.415197764374003</v>
+        <v>0.389691467414384</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))/H$40</f>
-        <v>0.286368043738465</v>
+        <v>0.285441388635265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -4899,27 +3974,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))/C$40</f>
-        <v>0.073024004903716</v>
+        <v>0.0736609039620186</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))/D$40</f>
-        <v>0.0760019204647085</v>
+        <v>0.0750810073979697</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))/E$40</f>
-        <v>0.0695538880800444</v>
+        <v>0.0752503981386747</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))/F$40</f>
-        <v>0.478414798276642</v>
+        <v>0.490467036393738</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))/G$40</f>
-        <v>0.19021356623412</v>
+        <v>0.192275358077921</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))/H$40</f>
-        <v>0.529671732023488</v>
+        <v>0.53707525043924</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
@@ -4931,27 +4006,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))</f>
-        <v>2.36341119024112</v>
+        <v>2.37567803631871</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))</f>
-        <v>2.42120020626942</v>
+        <v>2.40321025219694</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))</f>
-        <v>2.29742705051583</v>
+        <v>2.40651119006961</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))</f>
-        <v>1.89132405873603</v>
+        <v>1.84484858490994</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))</f>
-        <v>2.17929260626003</v>
+        <v>2.32193284610409</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))</f>
-        <v>1.88796180641873</v>
+        <v>1.86193647758329</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -4966,27 +4041,27 @@
       </c>
       <c r="C41" s="29" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.568774982970208</v>
+        <v>0.5727445105277</v>
       </c>
       <c r="D41" s="29" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.545877281231806</v>
+        <v>0.533384822206572</v>
       </c>
       <c r="E41" s="29" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.530437041847035</v>
+        <v>0.564791727242991</v>
       </c>
       <c r="F41" s="29" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.545747621264309</v>
+        <v>0.517672635586932</v>
       </c>
       <c r="G41" s="29" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.602374689383432</v>
+        <v>0.532211095802486</v>
       </c>
       <c r="H41" s="29" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.535374436778948</v>
+        <v>0.528959634182975</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -5015,34 +4090,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="42">
       <c r="A42" s="8" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C42" s="29" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.00246774267405272</v>
+        <v>0.0188910681754351</v>
       </c>
       <c r="D42" s="29" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0176161131635308</v>
+        <v>0.0179353998694569</v>
       </c>
       <c r="E42" s="29" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.00905572997406125</v>
+        <v>0.0131165311206132</v>
       </c>
       <c r="F42" s="29" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.0056929458770901</v>
+        <v>0.0142419328540564</v>
       </c>
       <c r="G42" s="29" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.00610422096215189</v>
+        <v>0.0134474491886795</v>
       </c>
       <c r="H42" s="29" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.00811042533256114</v>
+        <v>0.00886274316348136</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
@@ -5084,27 +4159,27 @@
       </c>
       <c r="C43" s="29" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.0123318939004093</v>
+        <v>0.00757666364312172</v>
       </c>
       <c r="D43" s="29" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.0118902016058564</v>
+        <v>0.00412195283919573</v>
       </c>
       <c r="E43" s="29" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.0101126185432076</v>
+        <v>0.00659120564348996</v>
       </c>
       <c r="F43" s="29" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.0036874820664525</v>
+        <v>0.00986874220892787</v>
       </c>
       <c r="G43" s="29" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0182121512666345</v>
+        <v>0.0198252796754241</v>
       </c>
       <c r="H43" s="29" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.00947502525523305</v>
+        <v>0.00470599039457738</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
@@ -5144,27 +4219,27 @@
       </c>
       <c r="C44" s="29" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.538542522899806</v>
+        <v>0.532509236494079</v>
       </c>
       <c r="D44" s="29" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.510629292773083</v>
+        <v>0.51918197392486</v>
       </c>
       <c r="E44" s="29" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.572059839619324</v>
+        <v>0.517603589035571</v>
       </c>
       <c r="F44" s="29" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.535721230916679</v>
+        <v>0.563054691534489</v>
       </c>
       <c r="G44" s="29" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.597764761187136</v>
+        <v>0.523584103100002</v>
       </c>
       <c r="H44" s="29" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.514979591378942</v>
+        <v>0.532101501589641</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
@@ -5204,27 +4279,27 @@
       </c>
       <c r="C45" s="29" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.551685485783964</v>
+        <v>0.54927128745243</v>
       </c>
       <c r="D45" s="29" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.558779057506472</v>
+        <v>0.518098150705919</v>
       </c>
       <c r="E45" s="29" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.599714750871062</v>
+        <v>0.511201909678057</v>
       </c>
       <c r="F45" s="29" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.527223442224786</v>
+        <v>0.605548810465261</v>
       </c>
       <c r="G45" s="29" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.547391032585874</v>
+        <v>0.560882199844345</v>
       </c>
       <c r="H45" s="29" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.561867601163685</v>
+        <v>0.55589298707433</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -5238,27 +4313,27 @@
       </c>
       <c r="C46" s="29" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.0122533806599677</v>
+        <v>0.0098753254301846</v>
       </c>
       <c r="D46" s="29" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.00232071986421943</v>
+        <v>0.00492512795142829</v>
       </c>
       <c r="E46" s="29" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.00728454351425171</v>
+        <v>0.019578854246065</v>
       </c>
       <c r="F46" s="29" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.00753527950495482</v>
+        <v>0.0172630802262574</v>
       </c>
       <c r="G46" s="29" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.00643220252357423</v>
+        <v>0.0186479751765728</v>
       </c>
       <c r="H46" s="29" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.00823727114126086</v>
+        <v>0.00633105702698231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -5268,27 +4343,27 @@
       </c>
       <c r="C47" s="29" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.0148718829546124</v>
+        <v>0.00533884041011333</v>
       </c>
       <c r="D47" s="29" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.00263268264010549</v>
+        <v>0.0111111981514841</v>
       </c>
       <c r="E47" s="29" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.019734385823831</v>
+        <v>0.0050411978084594</v>
       </c>
       <c r="F47" s="29" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.00918290878646076</v>
+        <v>0.0124007100146264</v>
       </c>
       <c r="G47" s="29" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.00593976491130888</v>
+        <v>0.0122237352095544</v>
       </c>
       <c r="H47" s="29" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.00683559841476381</v>
+        <v>0.00558323472738266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -5298,27 +4373,27 @@
       </c>
       <c r="C48" s="29" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.0113626054581255</v>
+        <v>0.0097101126704365</v>
       </c>
       <c r="D48" s="29" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.0084075075853616</v>
+        <v>0.0111148033849895</v>
       </c>
       <c r="E48" s="29" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.00445171157829464</v>
+        <v>0.00351863460615277</v>
       </c>
       <c r="F48" s="29" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.000418335432186723</v>
+        <v>0.00282664380036294</v>
       </c>
       <c r="G48" s="29" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.0141004534624517</v>
+        <v>0.00535673623904586</v>
       </c>
       <c r="H48" s="29" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.0105559325404465</v>
+        <v>0.0169660837948322</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -5328,27 +4403,27 @@
       </c>
       <c r="C49" s="29" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.00852876077406108</v>
+        <v>0.0116893869638443</v>
       </c>
       <c r="D49" s="29" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.00643234736286104</v>
+        <v>0.0129333998914808</v>
       </c>
       <c r="E49" s="29" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.00244613414630294</v>
+        <v>0.00108803663402796</v>
       </c>
       <c r="F49" s="29" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.0186413793172687</v>
+        <v>0.0182805926073343</v>
       </c>
       <c r="G49" s="29" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.0101198294293135</v>
+        <v>0.00280214210040867</v>
       </c>
       <c r="H49" s="29" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.000658285412937403</v>
+        <v>0.000913316309452057</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -5358,27 +4433,281 @@
       </c>
       <c r="C50" s="29" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.00811640457250178</v>
+        <v>0.00298658301122487</v>
       </c>
       <c r="D50" s="29" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.015335909081623</v>
+        <v>0.00728669071570039</v>
       </c>
       <c r="E50" s="29" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.00816431790590286</v>
+        <v>0.0170798556134105</v>
       </c>
       <c r="F50" s="29" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.00784603483974934</v>
+        <v>0.010998828727752</v>
       </c>
       <c r="G50" s="29" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.016549012856558</v>
+        <v>0.00412845497950912</v>
       </c>
       <c r="H50" s="29" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.000872418088838458</v>
+        <v>0.00228184484876692</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
+      <c r="B53" s="0" t="str">
+        <f aca="false">agent1!B53</f>
+        <v>weak ties fash</v>
+      </c>
+      <c r="J53" s="0" t="str">
+        <f aca="false">agent1!J53</f>
+        <v>beta_ik</v>
+      </c>
+      <c r="K53" s="0" t="str">
+        <f aca="false">agent1!K53</f>
+        <v>I=1</v>
+      </c>
+      <c r="L53" s="0" t="str">
+        <f aca="false">agent1!L53</f>
+        <v>I=2</v>
+      </c>
+      <c r="M53" s="0" t="str">
+        <f aca="false">agent1!M53</f>
+        <v>I=3</v>
+      </c>
+      <c r="O53" s="0" t="str">
+        <f aca="false">agent1!O53</f>
+        <v>B_ik</v>
+      </c>
+      <c r="P53" s="0" t="str">
+        <f aca="false">agent1!P53</f>
+        <v>I=1</v>
+      </c>
+      <c r="Q53" s="0" t="str">
+        <f aca="false">agent1!Q53</f>
+        <v>I=2</v>
+      </c>
+      <c r="R53" s="0" t="str">
+        <f aca="false">agent1!R53</f>
+        <v>I=2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="54">
+      <c r="B54" s="0" t="str">
+        <f aca="false">agent1!B54</f>
+        <v>#1 grumpy</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <f aca="false">agent1!C54</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <f aca="false">agent1!D54</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">agent1!E54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <f aca="false">agent1!F54</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">agent1!G54</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <f aca="false">agent1!H54</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <f aca="false">agent1!K54</f>
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <f aca="false">agent1!L54</f>
+        <v>0.5</v>
+      </c>
+      <c r="M54" s="0" t="n">
+        <f aca="false">agent1!M54</f>
+        <v>0.5</v>
+      </c>
+      <c r="P54" s="0" t="n">
+        <f aca="false">agent1!P54</f>
+        <v>1</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <f aca="false">agent1!Q54</f>
+        <v>1</v>
+      </c>
+      <c r="R54" s="0" t="n">
+        <f aca="false">agent1!R54</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="55">
+      <c r="B55" s="0" t="str">
+        <f aca="false">agent1!B55</f>
+        <v>#2 sleepy</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <f aca="false">agent1!C55</f>
+        <v>2</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <f aca="false">agent1!D55</f>
+        <v>2</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <f aca="false">agent1!E55</f>
+        <v>2</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <f aca="false">agent1!F55</f>
+        <v>2</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">agent1!G55</f>
+        <v>2</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <f aca="false">agent1!H55</f>
+        <v>2</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <f aca="false">agent1!K55</f>
+        <v>0</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <f aca="false">agent1!L55</f>
+        <v>0</v>
+      </c>
+      <c r="M55" s="0" t="n">
+        <f aca="false">agent1!M55</f>
+        <v>0</v>
+      </c>
+      <c r="P55" s="0" t="n">
+        <f aca="false">agent1!P55</f>
+        <v>1</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <f aca="false">agent1!Q55</f>
+        <v>1</v>
+      </c>
+      <c r="R55" s="0" t="n">
+        <f aca="false">agent1!R55</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="56">
+      <c r="B56" s="0" t="str">
+        <f aca="false">agent1!B56</f>
+        <v>#3 happy</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <f aca="false">agent1!C56</f>
+        <v>4</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <f aca="false">agent1!D56</f>
+        <v>4</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <f aca="false">agent1!E56</f>
+        <v>4</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <f aca="false">agent1!F56</f>
+        <v>4</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <f aca="false">agent1!G56</f>
+        <v>4</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <f aca="false">agent1!H56</f>
+        <v>4</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <f aca="false">agent1!K56</f>
+        <v>0.8</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <f aca="false">agent1!L56</f>
+        <v>0.8</v>
+      </c>
+      <c r="M56" s="0" t="n">
+        <f aca="false">agent1!M56</f>
+        <v>0.8</v>
+      </c>
+      <c r="P56" s="0" t="n">
+        <f aca="false">agent1!P56</f>
+        <v>1</v>
+      </c>
+      <c r="Q56" s="0" t="n">
+        <f aca="false">agent1!Q56</f>
+        <v>1</v>
+      </c>
+      <c r="R56" s="0" t="n">
+        <f aca="false">agent1!R56</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="57">
+      <c r="B57" s="0" t="str">
+        <f aca="false">agent1!B57</f>
+        <v>#4 sneezy</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <f aca="false">agent1!C57</f>
+        <v>1</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <f aca="false">agent1!D57</f>
+        <v>2</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">agent1!E57</f>
+        <v>2</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <f aca="false">agent1!F57</f>
+        <v>3</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">agent1!G57</f>
+        <v>4</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <f aca="false">agent1!H57</f>
+        <v>3</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <f aca="false">agent1!K57</f>
+        <v>0.3</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <f aca="false">agent1!L57</f>
+        <v>0.3</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <f aca="false">agent1!M57</f>
+        <v>0.3</v>
+      </c>
+      <c r="P57" s="0" t="n">
+        <f aca="false">agent1!P57</f>
+        <v>1</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <f aca="false">agent1!Q57</f>
+        <v>1</v>
+      </c>
+      <c r="R57" s="0" t="n">
+        <f aca="false">agent1!R57</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5397,19 +4726,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -5506,7 +4835,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
       <c r="A8" s="14"/>
       <c r="B8" s="9" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">$B$2*((C25*$B25)+(C26*$B26)+(C27*$B27)+(C28*$B28)+(C29*$B29))</f>
@@ -6550,27 +5879,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))/C$40</f>
-        <v>0.0987041524145507</v>
+        <v>0.105565609821025</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))/D$40</f>
-        <v>0.105713424360098</v>
+        <v>0.102730460146531</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))/E$40</f>
-        <v>0.102910124683828</v>
+        <v>0.0995802935862739</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))/F$40</f>
-        <v>0.0217464815622469</v>
+        <v>0.0164635218200502</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))/G$40</f>
-        <v>0.0307925619623999</v>
+        <v>0.0377958552379935</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))/H$40</f>
-        <v>0.017999658843852</v>
+        <v>0.0146276934818523</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -6582,27 +5911,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))/C$40</f>
-        <v>0.23805450739988</v>
+        <v>0.239700447354082</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))/D$40</f>
-        <v>0.23973146966223</v>
+        <v>0.239069936302101</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))/E$40</f>
-        <v>0.239111921562219</v>
+        <v>0.238287821378274</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))/F$40</f>
-        <v>0.0564244194939039</v>
+        <v>0.0471155483587553</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))/G$40</f>
-        <v>0.091700707308299</v>
+        <v>0.101817017227109</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))/H$40</f>
-        <v>0.0480069940961517</v>
+        <v>0.0418986561368466</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -6613,27 +5942,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))/C$40</f>
-        <v>0.393071225669477</v>
+        <v>0.377810099862226</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))/D$40</f>
-        <v>0.377489349165895</v>
+        <v>0.384026374316791</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))/E$40</f>
-        <v>0.383628779101515</v>
+        <v>0.391080707040686</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))/F$40</f>
-        <v>0.137772182140126</v>
+        <v>0.126075569566335</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))/G$40</f>
-        <v>0.244401967487129</v>
+        <v>0.247918526960781</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))/H$40</f>
-        <v>0.120545106167448</v>
+        <v>0.112459809927576</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -6644,27 +5973,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))/C$40</f>
-        <v>0.192124764795404</v>
+        <v>0.193453140510791</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))/D$40</f>
-        <v>0.193478177439188</v>
+        <v>0.19294427895263</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))/E$40</f>
-        <v>0.192978163663796</v>
+        <v>0.192313063659021</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))/F$40</f>
-        <v>0.307036301196551</v>
+        <v>0.305139060290627</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))/G$40</f>
-        <v>0.435857204135369</v>
+        <v>0.412382959680315</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))/H$40</f>
-        <v>0.27794756150632</v>
+        <v>0.275359059044823</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -6673,27 +6002,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))/C$40</f>
-        <v>0.0780453497206888</v>
+        <v>0.0834707024518767</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))/D$40</f>
-        <v>0.0835875793725893</v>
+        <v>0.0812289502819474</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))/E$40</f>
-        <v>0.0813710109886424</v>
+        <v>0.0787381143357442</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))/F$40</f>
-        <v>0.477020615607172</v>
+        <v>0.505206299964233</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))/G$40</f>
-        <v>0.197247559106803</v>
+        <v>0.200085640893801</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))/H$40</f>
-        <v>0.535500679386229</v>
+        <v>0.555654781408902</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
@@ -6705,27 +6034,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))</f>
-        <v>2.30196808859475</v>
+        <v>2.39495296278718</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))</f>
-        <v>2.39698794160762</v>
+        <v>2.35618561263071</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))</f>
-        <v>2.35862757782445</v>
+        <v>2.31368462249871</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))</f>
-        <v>1.89685180982009</v>
+        <v>1.79102560300618</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))</f>
-        <v>2.07599509529946</v>
+        <v>2.19416781609357</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))</f>
-        <v>1.86741126294399</v>
+        <v>1.79967856564543</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -6740,27 +6069,27 @@
       </c>
       <c r="C41" s="34" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.602744834078476</v>
+        <v>0.587369694560766</v>
       </c>
       <c r="D41" s="34" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.590427946485579</v>
+        <v>0.544397539226338</v>
       </c>
       <c r="E41" s="34" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.577416131645441</v>
+        <v>0.647697350056842</v>
       </c>
       <c r="F41" s="34" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.591282799327746</v>
+        <v>0.584949338948354</v>
       </c>
       <c r="G41" s="34" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.5972358006984</v>
+        <v>0.56639844905585</v>
       </c>
       <c r="H41" s="34" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.624183680303395</v>
+        <v>0.535353567777202</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -6789,34 +6118,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="42">
       <c r="A42" s="8" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C42" s="34" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.0830202524084598</v>
+        <v>0.0914905200712383</v>
       </c>
       <c r="D42" s="34" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0587753511965275</v>
+        <v>0.0495446916203946</v>
       </c>
       <c r="E42" s="34" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.0330264781136066</v>
+        <v>0.0493697906844318</v>
       </c>
       <c r="F42" s="34" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.00527881029993296</v>
+        <v>0.0563071182463318</v>
       </c>
       <c r="G42" s="34" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.0608670283574611</v>
+        <v>0.045646085171029</v>
       </c>
       <c r="H42" s="34" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.00352874542586505</v>
+        <v>0.0778073340188712</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
@@ -6858,27 +6187,27 @@
       </c>
       <c r="C43" s="34" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.0580584730021656</v>
+        <v>0.027797977020964</v>
       </c>
       <c r="D43" s="34" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.00351083222776651</v>
+        <v>0.0878616677597165</v>
       </c>
       <c r="E43" s="34" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.0356904822401702</v>
+        <v>0.0905934318434447</v>
       </c>
       <c r="F43" s="34" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.0702891437336803</v>
+        <v>0.0996954178903252</v>
       </c>
       <c r="G43" s="34" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0967177288141102</v>
+        <v>0.0899193305987865</v>
       </c>
       <c r="H43" s="34" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.0862896294333041</v>
+        <v>0.0758122716099024</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
@@ -6918,27 +6247,27 @@
       </c>
       <c r="C44" s="34" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.60149116110988</v>
+        <v>0.555001680320129</v>
       </c>
       <c r="D44" s="34" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.554022933635861</v>
+        <v>0.573955103708431</v>
       </c>
       <c r="E44" s="34" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.572743630548939</v>
+        <v>0.595434674015269</v>
       </c>
       <c r="F44" s="34" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.54059372371994</v>
+        <v>0.604199252557009</v>
       </c>
       <c r="G44" s="34" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.678500398714095</v>
+        <v>0.608852259535342</v>
       </c>
       <c r="H44" s="34" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.555769690359011</v>
+        <v>0.602071289392188</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
@@ -6978,27 +6307,27 @@
       </c>
       <c r="C45" s="34" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.620049976976588</v>
+        <v>0.554697990976274</v>
       </c>
       <c r="D45" s="34" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.588572776736692</v>
+        <v>0.527075727330521</v>
       </c>
       <c r="E45" s="34" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.642954295454547</v>
+        <v>0.564808303117752</v>
       </c>
       <c r="F45" s="34" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.540412498824298</v>
+        <v>0.614664399018511</v>
       </c>
       <c r="G45" s="34" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.611212858324871</v>
+        <v>0.619151162123308</v>
       </c>
       <c r="H45" s="34" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.600915623595938</v>
+        <v>0.556820171559229</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -7012,27 +6341,27 @@
       </c>
       <c r="C46" s="34" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.0187642508652061</v>
+        <v>0.0134100682567805</v>
       </c>
       <c r="D46" s="34" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.0490911838132888</v>
+        <v>0.0717709680553526</v>
       </c>
       <c r="E46" s="34" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.0897262067999691</v>
+        <v>0.0699985424987972</v>
       </c>
       <c r="F46" s="34" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.0347299406304956</v>
+        <v>0.0481394584290683</v>
       </c>
       <c r="G46" s="34" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.0580751593224704</v>
+        <v>0.00344002698548138</v>
       </c>
       <c r="H46" s="34" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.0714145719539374</v>
+        <v>0.0937018787488341</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -7042,27 +6371,27 @@
       </c>
       <c r="C47" s="34" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.0828566430602223</v>
+        <v>0.059789690002799</v>
       </c>
       <c r="D47" s="34" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.00824549053795636</v>
+        <v>0.0949305470567197</v>
       </c>
       <c r="E47" s="34" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.0274623518809676</v>
+        <v>0.0432465704157949</v>
       </c>
       <c r="F47" s="34" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.0441467586904764</v>
+        <v>0.00915948068723083</v>
       </c>
       <c r="G47" s="34" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.0570877508725971</v>
+        <v>0.0512376653030515</v>
       </c>
       <c r="H47" s="34" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.0294246757868677</v>
+        <v>0.0888926555868238</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -7072,27 +6401,27 @@
       </c>
       <c r="C48" s="34" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.035135698877275</v>
+        <v>0.0869668147526682</v>
       </c>
       <c r="D48" s="34" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.0401080032810569</v>
+        <v>0.0790356423240155</v>
       </c>
       <c r="E48" s="34" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.0882000269833952</v>
+        <v>0.0767543233465403</v>
       </c>
       <c r="F48" s="34" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.0681621769908816</v>
+        <v>0.0775602465961129</v>
       </c>
       <c r="G48" s="34" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.0453868135809898</v>
+        <v>0.0787310602143407</v>
       </c>
       <c r="H48" s="34" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.0490670553874224</v>
+        <v>0.0666736539453268</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -7102,27 +6431,27 @@
       </c>
       <c r="C49" s="34" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.0716909224167466</v>
+        <v>0.0533725182060152</v>
       </c>
       <c r="D49" s="34" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.00344528658315539</v>
+        <v>0.0886423123534769</v>
       </c>
       <c r="E49" s="34" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.052577887615189</v>
+        <v>0.0114603928290308</v>
       </c>
       <c r="F49" s="34" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.00738140470348299</v>
+        <v>0.0785166341811419</v>
       </c>
       <c r="G49" s="34" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.0737344303168356</v>
+        <v>0.0905739237554371</v>
       </c>
       <c r="H49" s="34" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.0492956164758653</v>
+        <v>0.0730790319852531</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -7132,27 +6461,281 @@
       </c>
       <c r="C50" s="34" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.0936710341367871</v>
+        <v>0.0817062981426716</v>
       </c>
       <c r="D50" s="34" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.047315001161769</v>
+        <v>0.0165312765631825</v>
       </c>
       <c r="E50" s="34" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.0865953681990504</v>
+        <v>0.0617860781960189</v>
       </c>
       <c r="F50" s="34" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.0566402089782059</v>
+        <v>0.0451772496569902</v>
       </c>
       <c r="G50" s="34" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.0617171615827829</v>
+        <v>0.0722114871721715</v>
       </c>
       <c r="H50" s="34" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.0631252941209823</v>
+        <v>0.0651678058784455</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
+      <c r="B53" s="0" t="str">
+        <f aca="false">agent1!B53</f>
+        <v>weak ties fash</v>
+      </c>
+      <c r="J53" s="0" t="str">
+        <f aca="false">agent1!J53</f>
+        <v>beta_ik</v>
+      </c>
+      <c r="K53" s="0" t="str">
+        <f aca="false">agent1!K53</f>
+        <v>I=1</v>
+      </c>
+      <c r="L53" s="0" t="str">
+        <f aca="false">agent1!L53</f>
+        <v>I=2</v>
+      </c>
+      <c r="M53" s="0" t="str">
+        <f aca="false">agent1!M53</f>
+        <v>I=3</v>
+      </c>
+      <c r="O53" s="0" t="str">
+        <f aca="false">agent1!O53</f>
+        <v>B_ik</v>
+      </c>
+      <c r="P53" s="0" t="str">
+        <f aca="false">agent1!P53</f>
+        <v>I=1</v>
+      </c>
+      <c r="Q53" s="0" t="str">
+        <f aca="false">agent1!Q53</f>
+        <v>I=2</v>
+      </c>
+      <c r="R53" s="0" t="str">
+        <f aca="false">agent1!R53</f>
+        <v>I=2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="54">
+      <c r="B54" s="0" t="str">
+        <f aca="false">agent1!B54</f>
+        <v>#1 grumpy</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <f aca="false">agent1!C54</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <f aca="false">agent1!D54</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">agent1!E54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <f aca="false">agent1!F54</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">agent1!G54</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <f aca="false">agent1!H54</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <f aca="false">agent1!K54</f>
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <f aca="false">agent1!L54</f>
+        <v>0.5</v>
+      </c>
+      <c r="M54" s="0" t="n">
+        <f aca="false">agent1!M54</f>
+        <v>0.5</v>
+      </c>
+      <c r="P54" s="0" t="n">
+        <f aca="false">agent1!P54</f>
+        <v>1</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <f aca="false">agent1!Q54</f>
+        <v>1</v>
+      </c>
+      <c r="R54" s="0" t="n">
+        <f aca="false">agent1!R54</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="55">
+      <c r="B55" s="0" t="str">
+        <f aca="false">agent1!B55</f>
+        <v>#2 sleepy</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <f aca="false">agent1!C55</f>
+        <v>2</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <f aca="false">agent1!D55</f>
+        <v>2</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <f aca="false">agent1!E55</f>
+        <v>2</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <f aca="false">agent1!F55</f>
+        <v>2</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">agent1!G55</f>
+        <v>2</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <f aca="false">agent1!H55</f>
+        <v>2</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <f aca="false">agent1!K55</f>
+        <v>0</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <f aca="false">agent1!L55</f>
+        <v>0</v>
+      </c>
+      <c r="M55" s="0" t="n">
+        <f aca="false">agent1!M55</f>
+        <v>0</v>
+      </c>
+      <c r="P55" s="0" t="n">
+        <f aca="false">agent1!P55</f>
+        <v>1</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <f aca="false">agent1!Q55</f>
+        <v>1</v>
+      </c>
+      <c r="R55" s="0" t="n">
+        <f aca="false">agent1!R55</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="56">
+      <c r="B56" s="0" t="str">
+        <f aca="false">agent1!B56</f>
+        <v>#3 happy</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <f aca="false">agent1!C56</f>
+        <v>4</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <f aca="false">agent1!D56</f>
+        <v>4</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <f aca="false">agent1!E56</f>
+        <v>4</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <f aca="false">agent1!F56</f>
+        <v>4</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <f aca="false">agent1!G56</f>
+        <v>4</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <f aca="false">agent1!H56</f>
+        <v>4</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <f aca="false">agent1!K56</f>
+        <v>0.8</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <f aca="false">agent1!L56</f>
+        <v>0.8</v>
+      </c>
+      <c r="M56" s="0" t="n">
+        <f aca="false">agent1!M56</f>
+        <v>0.8</v>
+      </c>
+      <c r="P56" s="0" t="n">
+        <f aca="false">agent1!P56</f>
+        <v>1</v>
+      </c>
+      <c r="Q56" s="0" t="n">
+        <f aca="false">agent1!Q56</f>
+        <v>1</v>
+      </c>
+      <c r="R56" s="0" t="n">
+        <f aca="false">agent1!R56</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="57">
+      <c r="B57" s="0" t="str">
+        <f aca="false">agent1!B57</f>
+        <v>#4 sneezy</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <f aca="false">agent1!C57</f>
+        <v>1</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <f aca="false">agent1!D57</f>
+        <v>2</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">agent1!E57</f>
+        <v>2</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <f aca="false">agent1!F57</f>
+        <v>3</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">agent1!G57</f>
+        <v>4</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <f aca="false">agent1!H57</f>
+        <v>3</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <f aca="false">agent1!K57</f>
+        <v>0.3</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <f aca="false">agent1!L57</f>
+        <v>0.3</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <f aca="false">agent1!M57</f>
+        <v>0.3</v>
+      </c>
+      <c r="P57" s="0" t="n">
+        <f aca="false">agent1!P57</f>
+        <v>1</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <f aca="false">agent1!Q57</f>
+        <v>1</v>
+      </c>
+      <c r="R57" s="0" t="n">
+        <f aca="false">agent1!R57</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7163,6 +6746,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
weak ties seem to work.
</commit_message>
<xml_diff>
--- a/BuyingJeans.Hw5.xlsx
+++ b/BuyingJeans.Hw5.xlsx
@@ -21,18 +21,18 @@
     <definedName function="false" hidden="false" name="__shared_1_0_5" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_6" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_7" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_11" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_12" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!)))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_18" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$K$42*POWER(ABS(A$15-$B1),$P$42)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42))))))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_20" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_21" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_22" vbProcedure="false">0.5+0.1*RAND()</definedName>
@@ -45,18 +45,18 @@
     <definedName function="false" hidden="false" name="__shared_2_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!)))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43))))))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_0" vbProcedure="false">$B$2*((A18*$B18)+(A19*$B19)+(A20*$B20)+(A21*$B21)+(A22*$B22))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_1" vbProcedure="false">(1/$B$2)*#REF!</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_2" vbProcedure="false">1/(1+EXP(($B$5*POWER(A$3/($B$4-A$3),$B$6))+($B$9*POWER(ABS(1-($B$2*A$8)),$B$10))-2))</definedName>
@@ -66,18 +66,18 @@
     <definedName function="false" hidden="false" name="__shared_3_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!)))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44))))))))))))))))))))))</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -651,12 +651,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0666666666667"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1137254901961"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -1804,27 +1804,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(C$15-$B35),$P$42)))/C$40</f>
-        <v>0.108297176141735</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(D$15-$B35),$P$42)))/D$40</f>
-        <v>0.116004803771132</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(E$15-$B35),$P$42)))/E$40</f>
-        <v>0.108717906802216</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(F$15-$B35),$P$42)))/F$40</f>
-        <v>0.00565197185505001</v>
+        <v>0.0472508813369664</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(G$15-$B35),$P$42)))/G$40</f>
-        <v>0.0252634565894201</v>
+        <v>0.104383474272034</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(H$15-$B35),$P$42)))/H$40</f>
-        <v>0.00219664127134893</v>
+        <v>0.0232965452072703</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="23"/>
@@ -1850,27 +1850,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(C$15-$B36),$P$42)))/C$40</f>
-        <v>0.369365318897504</v>
+        <v>0.380335995934576</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(D$15-$B36),$P$42)))/D$40</f>
-        <v>0.372921835158266</v>
+        <v>0.380335995934576</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(E$15-$B36),$P$42)))/E$40</f>
-        <v>0.369574889918842</v>
+        <v>0.380335995934576</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(F$15-$B36),$P$42)))/F$40</f>
-        <v>0.0294407474411251</v>
+        <v>0.111042237675138</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(G$15-$B36),$P$42)))/G$40</f>
-        <v>0.11284310510453</v>
+        <v>0.216852149768104</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(H$15-$B36),$P$42)))/H$40</f>
-        <v>0.0124428905252412</v>
+        <v>0.0599885945163799</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="23"/>
@@ -1895,27 +1895,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(C$15-$B37),$P$42)))/C$40</f>
-        <v>0.392315932701291</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(D$15-$B37),$P$42)))/D$40</f>
-        <v>0.37843469508647</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(E$15-$B37),$P$42)))/E$40</f>
-        <v>0.391538267528497</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(F$15-$B37),$P$42)))/F$40</f>
-        <v>0.128671843617798</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(G$15-$B37),$P$42)))/G$40</f>
-        <v>0.370844965054964</v>
+        <v>0.357528751919723</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(H$15-$B37),$P$42)))/H$40</f>
-        <v>0.061084660085764</v>
+        <v>0.140976582480673</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="23"/>
@@ -1940,27 +1940,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(C$15-$B38),$P$42)))/C$40</f>
-        <v>0.107839257836182</v>
+        <v>0.111042237675138</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(D$15-$B38),$P$42)))/D$40</f>
-        <v>0.108877612154849</v>
+        <v>0.111042237675138</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(E$15-$B38),$P$42)))/E$40</f>
-        <v>0.107900443828068</v>
+        <v>0.111042237675138</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(F$15-$B38),$P$42)))/F$40</f>
-        <v>0.414655762351118</v>
+        <v>0.380335995934576</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(G$15-$B38),$P$42)))/G$40</f>
-        <v>0.382777220489239</v>
+        <v>0.216852149768104</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(H$15-$B38),$P$42)))/H$40</f>
-        <v>0.246464634505995</v>
+        <v>0.292872748211301</v>
       </c>
       <c r="J38" s="23"/>
       <c r="K38" s="16"/>
@@ -1984,27 +1984,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(C$15-$B39),$P$42)))/C$40</f>
-        <v>0.0221823144232878</v>
+        <v>0.0472508813369664</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(D$15-$B39),$P$42)))/D$40</f>
-        <v>0.0237610538292827</v>
+        <v>0.0472508813369664</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(E$15-$B39),$P$42)))/E$40</f>
-        <v>0.0222684919223769</v>
+        <v>0.0472508813369664</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(F$15-$B39),$P$42)))/F$40</f>
-        <v>0.421579674734909</v>
+        <v>0.23068544252666</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(G$15-$B39),$P$42)))/G$40</f>
-        <v>0.108271252761848</v>
+        <v>0.104383474272034</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(H$15-$B39),$P$42)))/H$40</f>
-        <v>0.67781117361165</v>
+        <v>0.482865529584376</v>
       </c>
       <c r="J39" s="23"/>
       <c r="K39" s="16"/>
@@ -2031,27 +2031,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(C$15-$B35),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(C$15-$B36),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(C$15-$B37),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(C$15-$B38),$P$42)))+EXP((-C$41*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(C$15-$B39),$P$42)))</f>
-        <v>1.5460260702041</v>
+        <v>2.62925416129168</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(D$15-$B35),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(D$15-$B36),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(D$15-$B37),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(D$15-$B38),$P$42)))+EXP((-D$41*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(D$15-$B39),$P$42)))</f>
-        <v>1.60273534004076</v>
+        <v>2.62925416129168</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(E$15-$B35),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(E$15-$B36),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(E$15-$B37),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(E$15-$B38),$P$42)))+EXP((-E$41*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(E$15-$B39),$P$42)))</f>
-        <v>1.54909675506619</v>
+        <v>2.62925416129168</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(F$15-$B35),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(F$15-$B36),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(F$15-$B37),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(F$15-$B38),$P$42)))+EXP((-F$41*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(F$15-$B39),$P$42)))</f>
-        <v>1.43870944464774</v>
+        <v>2.62925416129168</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(G$15-$B35),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(G$15-$B36),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(G$15-$B37),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(G$15-$B38),$P$42)))+EXP((-G$41*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(G$15-$B39),$P$42)))</f>
-        <v>1.58455265163744</v>
+        <v>2.79697785039826</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$K$42*POWER(ABS(H$15-$B35),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$K$42*POWER(ABS(H$15-$B36),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$K$42*POWER(ABS(H$15-$B37),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$K$42*POWER(ABS(H$15-$B38),$P$42)))+EXP((-H$41*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$K$42*POWER(ABS(H$15-$B39),$P$42)))</f>
-        <v>1.47533714245458</v>
+        <v>2.07096994656203</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -2080,28 +2080,22 @@
         <v>36</v>
       </c>
       <c r="C41" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.560281287552789</v>
+        <v>0</v>
       </c>
       <c r="D41" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.514674681425095</v>
+        <v>0</v>
       </c>
       <c r="E41" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.557729857647791</v>
+        <v>0</v>
       </c>
       <c r="F41" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.516560098528862</v>
+        <v>0</v>
       </c>
       <c r="G41" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.531669058883563</v>
+        <v>0</v>
       </c>
       <c r="H41" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.511650231527165</v>
+        <v>0</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -2158,10 +2152,10 @@
         <v>0.5</v>
       </c>
       <c r="L42" s="15" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M42" s="15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O42" s="9" t="s">
         <v>43</v>
@@ -2203,7 +2197,7 @@
         <v>45</v>
       </c>
       <c r="K43" s="15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="15" t="n">
         <v>0.1</v>
@@ -2230,34 +2224,28 @@
         <v>46</v>
       </c>
       <c r="C44" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.512786097778007</v>
+        <v>0</v>
       </c>
       <c r="D44" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.50205766283907</v>
+        <v>0</v>
       </c>
       <c r="E44" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.510215834248811</v>
+        <v>0</v>
       </c>
       <c r="F44" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.549331844318658</v>
+        <v>0</v>
       </c>
       <c r="G44" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.516831900319085</v>
+        <v>0</v>
       </c>
       <c r="H44" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.524025741405785</v>
+        <v>0</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="K44" s="15" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L44" s="15" t="n">
         <v>0.1</v>
@@ -2284,28 +2272,22 @@
         <v>48</v>
       </c>
       <c r="C45" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.544786738837138</v>
+        <v>0</v>
       </c>
       <c r="D45" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.50193161140196</v>
+        <v>0</v>
       </c>
       <c r="E45" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.50318966396153</v>
+        <v>0</v>
       </c>
       <c r="F45" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.588707046210766</v>
+        <v>0</v>
       </c>
       <c r="G45" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.555680210608989</v>
+        <v>0</v>
       </c>
       <c r="H45" s="15" t="n">
-        <f aca="true">0.5+0.1*RAND()</f>
-        <v>0.553438443923369</v>
+        <v>0</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -2437,7 +2419,7 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
       <c r="B53" s="0" t="s">
         <v>55</v>
       </c>
@@ -2489,13 +2471,13 @@
         <v>0</v>
       </c>
       <c r="K54" s="15" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L54" s="15" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M54" s="15" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P54" s="15" t="n">
         <v>1</v>
@@ -2571,13 +2553,13 @@
         <v>4</v>
       </c>
       <c r="K56" s="15" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L56" s="15" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M56" s="15" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="P56" s="15" t="n">
         <v>1</v>
@@ -2589,7 +2571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="57">
       <c r="B57" s="0" t="s">
         <v>64</v>
       </c>
@@ -2612,13 +2594,13 @@
         <v>3</v>
       </c>
       <c r="K57" s="15" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L57" s="15" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="M57" s="15" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="P57" s="15" t="n">
         <v>1</v>
@@ -2653,12 +2635,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0666666666667"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1137254901961"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -3851,27 +3833,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))/C$40</f>
-        <v>0.112065937450578</v>
+        <v>0.213242763657043</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))/D$40</f>
-        <v>0.114226448851697</v>
+        <v>0.213978195434274</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))/E$40</f>
-        <v>0.114484155873081</v>
+        <v>0.214321911146214</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))/F$40</f>
-        <v>0.0165092751236266</v>
+        <v>0.136882834809335</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))/G$40</f>
-        <v>0.0458684654717235</v>
+        <v>0.172931720359786</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))/H$40</f>
-        <v>0.0145514355668166</v>
+        <v>0.117748743962133</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -3883,27 +3865,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))/C$40</f>
-        <v>0.247142021389393</v>
+        <v>0.24162278982991</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))/D$40</f>
-        <v>0.247588441214255</v>
+        <v>0.241437058319261</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))/E$40</f>
-        <v>0.247639393681416</v>
+        <v>0.241349708923177</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))/F$40</f>
-        <v>0.0498127716687151</v>
+        <v>0.177249411302609</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))/G$40</f>
-        <v>0.117035220682432</v>
+        <v>0.208916288420154</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))/H$40</f>
-        <v>0.0437266196936159</v>
+        <v>0.15804240961237</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -3914,27 +3896,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))/C$40</f>
-        <v>0.380875440275599</v>
+        <v>0.222873855299522</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))/D$40</f>
-        <v>0.376511966528432</v>
+        <v>0.221980730349763</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))/E$40</f>
-        <v>0.375995516567611</v>
+        <v>0.221564269660894</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))/F$40</f>
-        <v>0.134531460234398</v>
+        <v>0.217161246162058</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))/G$40</f>
-        <v>0.25512948835354</v>
+        <v>0.232180506854759</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))/H$40</f>
-        <v>0.119205305665062</v>
+        <v>0.202886830897005</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -3945,27 +3927,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))/C$40</f>
-        <v>0.186255696922411</v>
+        <v>0.182096192541859</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))/D$40</f>
-        <v>0.186592136007647</v>
+        <v>0.181956218158863</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))/E$40</f>
-        <v>0.186630535739217</v>
+        <v>0.181890388307056</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))/F$40</f>
-        <v>0.308679456579522</v>
+        <v>0.244417540096775</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))/G$40</f>
-        <v>0.389691467414384</v>
+        <v>0.210991358068221</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))/H$40</f>
-        <v>0.285441388635265</v>
+        <v>0.246464136654958</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -3974,27 +3956,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))/C$40</f>
-        <v>0.0736609039620186</v>
+        <v>0.140164398671666</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))/D$40</f>
-        <v>0.0750810073979697</v>
+        <v>0.140647797737838</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))/E$40</f>
-        <v>0.0752503981386747</v>
+        <v>0.14087372196266</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))/F$40</f>
-        <v>0.490467036393738</v>
+        <v>0.224288967629223</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))/G$40</f>
-        <v>0.192275358077921</v>
+        <v>0.17498012629708</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))/H$40</f>
-        <v>0.53707525043924</v>
+        <v>0.274857878873534</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
@@ -4006,27 +3988,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))</f>
-        <v>2.37567803631871</v>
+        <v>4.05986344526568</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))</f>
-        <v>2.40321025219694</v>
+        <v>4.07619804029952</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))</f>
-        <v>2.40651119006961</v>
+        <v>4.08385981828578</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))</f>
-        <v>1.84484858490994</v>
+        <v>4.03424844119736</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))</f>
-        <v>2.32193284610409</v>
+        <v>4.28850463981276</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))</f>
-        <v>1.86193647758329</v>
+        <v>3.63824389571206</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -4041,27 +4023,27 @@
       </c>
       <c r="C41" s="29" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.5727445105277</v>
+        <v>0.00199418325908482</v>
       </c>
       <c r="D41" s="29" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.533384822206572</v>
+        <v>0.0130933519080281</v>
       </c>
       <c r="E41" s="29" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.564791727242991</v>
+        <v>0.000763714741915464</v>
       </c>
       <c r="F41" s="29" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.517672635586932</v>
+        <v>0.00343534072861075</v>
       </c>
       <c r="G41" s="29" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.532211095802486</v>
+        <v>0.000169509891420603</v>
       </c>
       <c r="H41" s="29" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.528959634182975</v>
+        <v>0.0166863788664341</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -4097,27 +4079,27 @@
       </c>
       <c r="C42" s="29" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.0188910681754351</v>
+        <v>0.00872516953386366</v>
       </c>
       <c r="D42" s="29" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0179353998694569</v>
+        <v>0.0172594982665032</v>
       </c>
       <c r="E42" s="29" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.0131165311206132</v>
+        <v>0.000100273285061121</v>
       </c>
       <c r="F42" s="29" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.0142419328540564</v>
+        <v>0.0123086791764945</v>
       </c>
       <c r="G42" s="29" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.0134474491886795</v>
+        <v>0.0194610762968659</v>
       </c>
       <c r="H42" s="29" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.00886274316348136</v>
+        <v>0.00824648159556091</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
@@ -4128,11 +4110,11 @@
       </c>
       <c r="L42" s="29" t="n">
         <f aca="false">agent1!L42</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M42" s="29" t="n">
         <f aca="false">agent1!M42</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O42" s="9" t="s">
         <v>43</v>
@@ -4159,34 +4141,34 @@
       </c>
       <c r="C43" s="29" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.00757666364312172</v>
+        <v>0.013555175466463</v>
       </c>
       <c r="D43" s="29" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.00412195283919573</v>
+        <v>0.00714858678169549</v>
       </c>
       <c r="E43" s="29" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.00659120564348996</v>
+        <v>0.00551540325395763</v>
       </c>
       <c r="F43" s="29" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.00986874220892787</v>
+        <v>0.0180970652773976</v>
       </c>
       <c r="G43" s="29" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0198252796754241</v>
+        <v>0.0120156239625067</v>
       </c>
       <c r="H43" s="29" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.00470599039457738</v>
+        <v>0.0146372821927071</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
       </c>
       <c r="K43" s="29" t="n">
         <f aca="false">agent1!K43</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="29" t="n">
         <f aca="false">agent1!L43</f>
@@ -4219,34 +4201,34 @@
       </c>
       <c r="C44" s="29" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.532509236494079</v>
+        <v>0.0192281497269869</v>
       </c>
       <c r="D44" s="29" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.51918197392486</v>
+        <v>0.0159817668329924</v>
       </c>
       <c r="E44" s="29" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.517603589035571</v>
+        <v>0.0144657478109002</v>
       </c>
       <c r="F44" s="29" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.563054691534489</v>
+        <v>0.0140572618227452</v>
       </c>
       <c r="G44" s="29" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.523584103100002</v>
+        <v>0.00430205968208611</v>
       </c>
       <c r="H44" s="29" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.532101501589641</v>
+        <v>0.00903766732662916</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="K44" s="29" t="n">
         <f aca="false">agent1!K44</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L44" s="29" t="n">
         <f aca="false">agent1!L44</f>
@@ -4279,27 +4261,27 @@
       </c>
       <c r="C45" s="29" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.54927128745243</v>
+        <v>0.00735592100769281</v>
       </c>
       <c r="D45" s="29" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.518098150705919</v>
+        <v>0.00809176839888096</v>
       </c>
       <c r="E45" s="29" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.511201909678057</v>
+        <v>0.00392105360515416</v>
       </c>
       <c r="F45" s="29" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.605548810465261</v>
+        <v>0.0018128377571702</v>
       </c>
       <c r="G45" s="29" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.560882199844345</v>
+        <v>0.0165006668120623</v>
       </c>
       <c r="H45" s="29" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.55589298707433</v>
+        <v>0.0048676382098347</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -4313,27 +4295,27 @@
       </c>
       <c r="C46" s="29" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.0098753254301846</v>
+        <v>0.00264850493520498</v>
       </c>
       <c r="D46" s="29" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.00492512795142829</v>
+        <v>0.0157288165483624</v>
       </c>
       <c r="E46" s="29" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.019578854246065</v>
+        <v>0.000849405042827129</v>
       </c>
       <c r="F46" s="29" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.0172630802262574</v>
+        <v>0.0171142527554184</v>
       </c>
       <c r="G46" s="29" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.0186479751765728</v>
+        <v>0.00978607837110758</v>
       </c>
       <c r="H46" s="29" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.00633105702698231</v>
+        <v>0.00515146472491324</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -4343,27 +4325,27 @@
       </c>
       <c r="C47" s="29" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.00533884041011333</v>
+        <v>0.00615192008204758</v>
       </c>
       <c r="D47" s="29" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.0111111981514841</v>
+        <v>0.0117802616301924</v>
       </c>
       <c r="E47" s="29" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.0050411978084594</v>
+        <v>0.0182448166422546</v>
       </c>
       <c r="F47" s="29" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.0124007100146264</v>
+        <v>0.00691563482396305</v>
       </c>
       <c r="G47" s="29" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.0122237352095544</v>
+        <v>0.0152156023681164</v>
       </c>
       <c r="H47" s="29" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.00558323472738266</v>
+        <v>0.0184143265336752</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -4373,27 +4355,27 @@
       </c>
       <c r="C48" s="29" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.0097101126704365</v>
+        <v>0.00360201369971037</v>
       </c>
       <c r="D48" s="29" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.0111148033849895</v>
+        <v>0.00394077190198004</v>
       </c>
       <c r="E48" s="29" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.00351863460615277</v>
+        <v>0.0156738248001784</v>
       </c>
       <c r="F48" s="29" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.00282664380036294</v>
+        <v>0.00370228698477149</v>
       </c>
       <c r="G48" s="29" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.00535673623904586</v>
+        <v>0.0162494510784745</v>
       </c>
       <c r="H48" s="29" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.0169660837948322</v>
+        <v>0.0151349011063576</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -4403,27 +4385,27 @@
       </c>
       <c r="C49" s="29" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.0116893869638443</v>
+        <v>0.0119487685803324</v>
       </c>
       <c r="D49" s="29" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.0129333998914808</v>
+        <v>0.00980462655425072</v>
       </c>
       <c r="E49" s="29" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.00108803663402796</v>
+        <v>0.00228348788805306</v>
       </c>
       <c r="F49" s="29" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.0182805926073343</v>
+        <v>0.01746417183429</v>
       </c>
       <c r="G49" s="29" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.00280214210040867</v>
+        <v>0.00790169183164835</v>
       </c>
       <c r="H49" s="29" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.000913316309452057</v>
+        <v>0.0142991118505597</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -4433,27 +4415,27 @@
       </c>
       <c r="C50" s="29" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.00298658301122487</v>
+        <v>0.0121014540269971</v>
       </c>
       <c r="D50" s="29" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.00728669071570039</v>
+        <v>0.0152576128486544</v>
       </c>
       <c r="E50" s="29" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.0170798556134105</v>
+        <v>0.00239088024944067</v>
       </c>
       <c r="F50" s="29" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.010998828727752</v>
+        <v>0.0160225076321512</v>
       </c>
       <c r="G50" s="29" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.00412845497950912</v>
+        <v>0.0170704506058246</v>
       </c>
       <c r="H50" s="29" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.00228184484876692</v>
+        <v>0.0188915470615029</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
@@ -4525,15 +4507,15 @@
       </c>
       <c r="K54" s="0" t="n">
         <f aca="false">agent1!K54</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">agent1!L54</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M54" s="0" t="n">
         <f aca="false">agent1!M54</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P54" s="0" t="n">
         <f aca="false">agent1!P54</f>
@@ -4633,15 +4615,15 @@
       </c>
       <c r="K56" s="0" t="n">
         <f aca="false">agent1!K56</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L56" s="0" t="n">
         <f aca="false">agent1!L56</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M56" s="0" t="n">
         <f aca="false">agent1!M56</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="P56" s="0" t="n">
         <f aca="false">agent1!P56</f>
@@ -4687,15 +4669,15 @@
       </c>
       <c r="K57" s="0" t="n">
         <f aca="false">agent1!K57</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L57" s="0" t="n">
         <f aca="false">agent1!L57</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="M57" s="0" t="n">
         <f aca="false">agent1!M57</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="P57" s="0" t="n">
         <f aca="false">agent1!P57</f>
@@ -4733,12 +4715,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0666666666667"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1137254901961"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -5879,27 +5861,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))/C$40</f>
-        <v>0.105565609821025</v>
+        <v>0.207915113468915</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))/D$40</f>
-        <v>0.102730460146531</v>
+        <v>0.188162639784319</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))/E$40</f>
-        <v>0.0995802935862739</v>
+        <v>0.193447337411528</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))/F$40</f>
-        <v>0.0164635218200502</v>
+        <v>0.160875333369661</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))/G$40</f>
-        <v>0.0377958552379935</v>
+        <v>0.151050437541635</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))/H$40</f>
-        <v>0.0146276934818523</v>
+        <v>0.145158143046964</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -5911,27 +5893,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))/C$40</f>
-        <v>0.239700447354082</v>
+        <v>0.231112417866771</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))/D$40</f>
-        <v>0.239069936302101</v>
+        <v>0.23632860588477</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))/E$40</f>
-        <v>0.238287821378274</v>
+        <v>0.23506154549525</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))/F$40</f>
-        <v>0.0471155483587553</v>
+        <v>0.18392238272885</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))/G$40</f>
-        <v>0.101817017227109</v>
+        <v>0.191167582011692</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))/H$40</f>
-        <v>0.0418986561368466</v>
+        <v>0.170104722823743</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -5942,27 +5924,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))/C$40</f>
-        <v>0.377810099862226</v>
+        <v>0.210051970533556</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))/D$40</f>
-        <v>0.384026374316791</v>
+        <v>0.235996744893708</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))/E$40</f>
-        <v>0.391080707040686</v>
+        <v>0.228823094892995</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))/F$40</f>
-        <v>0.126075569566335</v>
+        <v>0.208803062107524</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))/G$40</f>
-        <v>0.247918526960781</v>
+        <v>0.235649888796073</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))/H$40</f>
-        <v>0.112459809927576</v>
+        <v>0.19806958607857</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -5973,27 +5955,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))/C$40</f>
-        <v>0.193453140510791</v>
+        <v>0.186522067609348</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))/D$40</f>
-        <v>0.19294427895263</v>
+        <v>0.19073185513672</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))/E$40</f>
-        <v>0.192313063659021</v>
+        <v>0.189709258749124</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))/F$40</f>
-        <v>0.305139060290627</v>
+        <v>0.233381851369678</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))/G$40</f>
-        <v>0.412382959680315</v>
+        <v>0.23194800333608</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))/H$40</f>
-        <v>0.275359059044823</v>
+        <v>0.228504892833997</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -6002,27 +5984,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))/C$40</f>
-        <v>0.0834707024518767</v>
+        <v>0.16439843052141</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))/D$40</f>
-        <v>0.0812289502819474</v>
+        <v>0.148780154300482</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))/E$40</f>
-        <v>0.0787381143357442</v>
+        <v>0.152958763451102</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))/F$40</f>
-        <v>0.505206299964233</v>
+        <v>0.213017370424287</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))/G$40</f>
-        <v>0.200085640893801</v>
+        <v>0.190184088314521</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))/H$40</f>
-        <v>0.555654781408902</v>
+        <v>0.258162655216726</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
@@ -6034,27 +6016,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))</f>
-        <v>2.39495296278718</v>
+        <v>4.3076835496357</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))</f>
-        <v>2.35618561263071</v>
+        <v>3.83410973928261</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))</f>
-        <v>2.31368462249871</v>
+        <v>3.95430984996987</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))</f>
-        <v>1.79102560300618</v>
+        <v>4.24771658871625</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))</f>
-        <v>2.19416781609357</v>
+        <v>3.90103559859016</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))</f>
-        <v>1.79967856564543</v>
+        <v>3.87352694044964</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -6069,27 +6051,27 @@
       </c>
       <c r="C41" s="34" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.587369694560766</v>
+        <v>0.0344550781417638</v>
       </c>
       <c r="D41" s="34" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.544397539226338</v>
+        <v>0.014925641939044</v>
       </c>
       <c r="E41" s="34" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.647697350056842</v>
+        <v>0.0809335181023926</v>
       </c>
       <c r="F41" s="34" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.584949338948354</v>
+        <v>0.0256791613530368</v>
       </c>
       <c r="G41" s="34" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.56639844905585</v>
+        <v>0.0495038160588592</v>
       </c>
       <c r="H41" s="34" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.535353567777202</v>
+        <v>0.0570115299429745</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -6125,27 +6107,27 @@
       </c>
       <c r="C42" s="34" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.0914905200712383</v>
+        <v>0.0177507940214127</v>
       </c>
       <c r="D42" s="34" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0495446916203946</v>
+        <v>0.0675138845574111</v>
       </c>
       <c r="E42" s="34" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.0493697906844318</v>
+        <v>0.0767153894528747</v>
       </c>
       <c r="F42" s="34" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.0563071182463318</v>
+        <v>0.0961199180223048</v>
       </c>
       <c r="G42" s="34" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.045646085171029</v>
+        <v>0.0860253194812685</v>
       </c>
       <c r="H42" s="34" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.0778073340188712</v>
+        <v>0.0579626448452473</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
@@ -6156,11 +6138,11 @@
       </c>
       <c r="L42" s="34" t="n">
         <f aca="false">agent1!L42</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M42" s="34" t="n">
         <f aca="false">agent1!M42</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O42" s="9" t="s">
         <v>43</v>
@@ -6187,34 +6169,34 @@
       </c>
       <c r="C43" s="34" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.027797977020964</v>
+        <v>0.0717944235540926</v>
       </c>
       <c r="D43" s="34" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.0878616677597165</v>
+        <v>0.0457691623829305</v>
       </c>
       <c r="E43" s="34" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.0905934318434447</v>
+        <v>0.00698577761650085</v>
       </c>
       <c r="F43" s="34" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.0996954178903252</v>
+        <v>0.083211862994358</v>
       </c>
       <c r="G43" s="34" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0899193305987865</v>
+        <v>0.0330900215543807</v>
       </c>
       <c r="H43" s="34" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.0758122716099024</v>
+        <v>0.0464942368213087</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
       </c>
       <c r="K43" s="34" t="n">
         <f aca="false">agent1!K43</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="34" t="n">
         <f aca="false">agent1!L43</f>
@@ -6247,34 +6229,34 @@
       </c>
       <c r="C44" s="34" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.555001680320129</v>
+        <v>0.00445072925649583</v>
       </c>
       <c r="D44" s="34" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.573955103708431</v>
+        <v>0.098594777751714</v>
       </c>
       <c r="E44" s="34" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.595434674015269</v>
+        <v>0.0731018180493265</v>
       </c>
       <c r="F44" s="34" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.604199252557009</v>
+        <v>0.00869775447063148</v>
       </c>
       <c r="G44" s="34" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.608852259535342</v>
+        <v>0.0841660415288061</v>
       </c>
       <c r="H44" s="34" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.602071289392188</v>
+        <v>0.0220322099048644</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="K44" s="34" t="n">
         <f aca="false">agent1!K44</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L44" s="34" t="n">
         <f aca="false">agent1!L44</f>
@@ -6307,27 +6289,27 @@
       </c>
       <c r="C45" s="34" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.554697990976274</v>
+        <v>0.0547074222471565</v>
       </c>
       <c r="D45" s="34" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.527075727330521</v>
+        <v>0.0935972916893661</v>
       </c>
       <c r="E45" s="34" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.564808303117752</v>
+        <v>0.0227823010645807</v>
       </c>
       <c r="F45" s="34" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.614664399018511</v>
+        <v>0.0666618234943599</v>
       </c>
       <c r="G45" s="34" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.619151162123308</v>
+        <v>0.0737098298966885</v>
       </c>
       <c r="H45" s="34" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.556820171559229</v>
+        <v>0.00813455409370363</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -6341,27 +6323,27 @@
       </c>
       <c r="C46" s="34" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.0134100682567805</v>
+        <v>0.0611195588484407</v>
       </c>
       <c r="D46" s="34" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.0717709680553526</v>
+        <v>0.0781605591531843</v>
       </c>
       <c r="E46" s="34" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.0699985424987972</v>
+        <v>0.00672933184541762</v>
       </c>
       <c r="F46" s="34" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.0481394584290683</v>
+        <v>0.0342213768977672</v>
       </c>
       <c r="G46" s="34" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.00344002698548138</v>
+        <v>0.0868583136238158</v>
       </c>
       <c r="H46" s="34" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.0937018787488341</v>
+        <v>0.0908953733742237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -6371,27 +6353,27 @@
       </c>
       <c r="C47" s="34" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.059789690002799</v>
+        <v>0.0562535868491977</v>
       </c>
       <c r="D47" s="34" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.0949305470567197</v>
+        <v>0.0213133917655796</v>
       </c>
       <c r="E47" s="34" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.0432465704157949</v>
+        <v>0.00582101531326771</v>
       </c>
       <c r="F47" s="34" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.00915948068723083</v>
+        <v>0.0371871049515903</v>
       </c>
       <c r="G47" s="34" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.0512376653030515</v>
+        <v>0.0469925531186163</v>
       </c>
       <c r="H47" s="34" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.0888926555868238</v>
+        <v>0.0553248314186931</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -6401,27 +6383,27 @@
       </c>
       <c r="C48" s="34" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.0869668147526682</v>
+        <v>0.0941986348945648</v>
       </c>
       <c r="D48" s="34" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.0790356423240155</v>
+        <v>0.0647433471400291</v>
       </c>
       <c r="E48" s="34" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.0767543233465403</v>
+        <v>0.0228387159761041</v>
       </c>
       <c r="F48" s="34" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.0775602465961129</v>
+        <v>0.0709140243474394</v>
       </c>
       <c r="G48" s="34" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.0787310602143407</v>
+        <v>0.0608632652089</v>
       </c>
       <c r="H48" s="34" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.0666736539453268</v>
+        <v>0.00886403550393879</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -6431,27 +6413,27 @@
       </c>
       <c r="C49" s="34" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.0533725182060152</v>
+        <v>0.0288766691926867</v>
       </c>
       <c r="D49" s="34" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.0886423123534769</v>
+        <v>0.0326576887629926</v>
       </c>
       <c r="E49" s="34" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.0114603928290308</v>
+        <v>0.0546331978868693</v>
       </c>
       <c r="F49" s="34" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.0785166341811419</v>
+        <v>0.0358624468557537</v>
       </c>
       <c r="G49" s="34" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.0905739237554371</v>
+        <v>0.0158695518039167</v>
       </c>
       <c r="H49" s="34" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.0730790319852531</v>
+        <v>0.0877232194878161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -6461,27 +6443,27 @@
       </c>
       <c r="C50" s="34" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.0817062981426716</v>
+        <v>0.0823566836770624</v>
       </c>
       <c r="D50" s="34" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.0165312765631825</v>
+        <v>0.0705769740510732</v>
       </c>
       <c r="E50" s="34" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.0617860781960189</v>
+        <v>0.0813205111771822</v>
       </c>
       <c r="F50" s="34" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.0451772496569902</v>
+        <v>0.00513898474164307</v>
       </c>
       <c r="G50" s="34" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.0722114871721715</v>
+        <v>0.0372387975919992</v>
       </c>
       <c r="H50" s="34" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.0651678058784455</v>
+        <v>0.0550303410738707</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
@@ -6553,15 +6535,15 @@
       </c>
       <c r="K54" s="0" t="n">
         <f aca="false">agent1!K54</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">agent1!L54</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M54" s="0" t="n">
         <f aca="false">agent1!M54</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P54" s="0" t="n">
         <f aca="false">agent1!P54</f>
@@ -6661,15 +6643,15 @@
       </c>
       <c r="K56" s="0" t="n">
         <f aca="false">agent1!K56</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L56" s="0" t="n">
         <f aca="false">agent1!L56</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M56" s="0" t="n">
         <f aca="false">agent1!M56</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="P56" s="0" t="n">
         <f aca="false">agent1!P56</f>
@@ -6715,15 +6697,15 @@
       </c>
       <c r="K57" s="0" t="n">
         <f aca="false">agent1!K57</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L57" s="0" t="n">
         <f aca="false">agent1!L57</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="M57" s="0" t="n">
         <f aca="false">agent1!M57</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="P57" s="0" t="n">
         <f aca="false">agent1!P57</f>

</xml_diff>

<commit_message>
model description documents (PDF) added
</commit_message>
<xml_diff>
--- a/BuyingJeans.Hw5.xlsx
+++ b/BuyingJeans.Hw5.xlsx
@@ -21,18 +21,18 @@
     <definedName function="false" hidden="false" name="__shared_1_0_5" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_6" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_7" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_8" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_9" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_10" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_11" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_12" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!)))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_15" vbProcedure="false">MAX(#REF!))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_18" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$K$42*POWER(ABS(A$15-$B1),$P$42)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_1_0_19" vbProcedure="false">EXP((-A$41*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))+EXP((-A$41*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$K$42*POWER(ABS(A$15-#REF!),$P$42)))))))))))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_20" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_21" vbProcedure="false">0.5+0.1*RAND()</definedName>
     <definedName function="false" hidden="false" name="__shared_1_0_22" vbProcedure="false">0.5+0.1*RAND()</definedName>
@@ -45,18 +45,18 @@
     <definedName function="false" hidden="false" name="__shared_2_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!)))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_15" vbProcedure="false">MAX(#REF!))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_2_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$L$43*POWER(ABS(A$15-$B1),$Q$43)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_2_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$L$43*POWER(ABS(A$15-#REF!),$Q$43)))))))))))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_0" vbProcedure="false">$B$2*((A18*$B18)+(A19*$B19)+(A20*$B20)+(A21*$B21)+(A22*$B22))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_1" vbProcedure="false">(1/$B$2)*#REF!</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_2" vbProcedure="false">1/(1+EXP(($B$5*POWER(A$3/($B$4-A$3),$B$6))+($B$9*POWER(ABS(1-($B$2*A$8)),$B$10))-2))</definedName>
@@ -66,18 +66,18 @@
     <definedName function="false" hidden="false" name="__shared_3_0_6" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_7" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*$K1)-A$15),$K$22))/A$21</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_8" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*$T1)-A$15),$T$22))/A$21</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_9" vbProcedure="false">EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-#REF!)),$B$22))+EXP(-$B$21*POWER(ABS($B$2*(A$15-$B1)),$B$22))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_10" vbProcedure="false">EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))+EXP(-$K$21*POWER(ABS(($B$2*#REF!)-A$15),$K$22))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_11" vbProcedure="false">EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))+EXP(-$T$21*POWER(ABS(($B$2*#REF!)-A$15),$T$22))))))))))))))))))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_12" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_13" vbProcedure="false">#REF!*#REF!*#REF!/A$30</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_14" vbProcedure="false">#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!+#REF!*#REF!*#REF!</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!)))))</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_15" vbProcedure="false">MAX(#REF!))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_16" vbProcedure="false">IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0)+IF(#REF!=A$31,#REF!,0))))))</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_17" vbProcedure="false">A$15</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_18" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
     <definedName function="false" hidden="false" name="__shared_3_0_19" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-$B1),$B$40))+(-$M$44*POWER(ABS(A$15-$B1),$R$44)))/A$40</definedName>
-    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44))))))))))))))))))))))</definedName>
+    <definedName function="false" hidden="false" name="__shared_3_0_20" vbProcedure="false">EXP((-A$44*POWER(ABS(MIN(A$15+1,4-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))+EXP((-A$44*POWER(ABS(MIN(A$15+1,4)-#REF!),$B$40))+(-$M$44*POWER(ABS(A$15-#REF!),$R$44)))))))))))))))))))))))))))</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -651,12 +651,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1137254901961"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.74901960784314"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -2164,10 +2164,10 @@
         <v>1.3</v>
       </c>
       <c r="Q42" s="15" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="15" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
@@ -2200,22 +2200,22 @@
         <v>0</v>
       </c>
       <c r="L43" s="15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O43" s="9" t="s">
         <v>45</v>
       </c>
       <c r="P43" s="15" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="Q43" s="15" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="R43" s="15" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="44">
@@ -2248,22 +2248,22 @@
         <v>0</v>
       </c>
       <c r="L44" s="15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="15" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="P44" s="15" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="15" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="R44" s="15" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="45">
@@ -2635,12 +2635,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1137254901961"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.74901960784314"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -3833,27 +3833,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))/C$40</f>
-        <v>0.213242763657043</v>
+        <v>0.199855285587182</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))/D$40</f>
-        <v>0.213978195434274</v>
+        <v>0.197060701189229</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))/E$40</f>
-        <v>0.214321911146214</v>
+        <v>0.199092955361461</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))/F$40</f>
-        <v>0.136882834809335</v>
+        <v>0.197737758285075</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))/G$40</f>
-        <v>0.172931720359786</v>
+        <v>0.194411990890113</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))/H$40</f>
-        <v>0.117748743962133</v>
+        <v>0.190261161166863</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -3865,27 +3865,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))/C$40</f>
-        <v>0.24162278982991</v>
+        <v>0.2000471417772</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))/D$40</f>
-        <v>0.241437058319261</v>
+        <v>0.200944343889655</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))/E$40</f>
-        <v>0.241349708923177</v>
+        <v>0.200294373840452</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))/F$40</f>
-        <v>0.177249411302609</v>
+        <v>0.198969480151996</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))/G$40</f>
-        <v>0.208916288420154</v>
+        <v>0.198151911897221</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))/H$40</f>
-        <v>0.15804240961237</v>
+        <v>0.195472270929014</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -3896,27 +3896,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))/C$40</f>
-        <v>0.222873855299522</v>
+        <v>0.200195145271237</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))/D$40</f>
-        <v>0.221980730349763</v>
+        <v>0.203989909842231</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))/E$40</f>
-        <v>0.221564269660894</v>
+        <v>0.201225341596174</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))/F$40</f>
-        <v>0.217161246162058</v>
+        <v>0.200127363423609</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))/G$40</f>
-        <v>0.232180506854759</v>
+        <v>0.201583530316864</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))/H$40</f>
-        <v>0.202886830897005</v>
+        <v>0.200470573850608</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -3927,27 +3927,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))/C$40</f>
-        <v>0.182096192541859</v>
+        <v>0.2000471417772</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))/D$40</f>
-        <v>0.181956218158863</v>
+        <v>0.200944343889655</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))/E$40</f>
-        <v>0.181890388307056</v>
+        <v>0.200294373840452</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))/F$40</f>
-        <v>0.244417540096775</v>
+        <v>0.201176499576094</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))/G$40</f>
-        <v>0.210991358068221</v>
+        <v>0.204269036578937</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))/H$40</f>
-        <v>0.246464136654958</v>
+        <v>0.205083913388127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -3956,27 +3956,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))/C$40</f>
-        <v>0.140164398671666</v>
+        <v>0.199855285587182</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))/D$40</f>
-        <v>0.140647797737838</v>
+        <v>0.197060701189229</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))/E$40</f>
-        <v>0.14087372196266</v>
+        <v>0.199092955361461</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))/F$40</f>
-        <v>0.224288967629223</v>
+        <v>0.201988898563227</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))/G$40</f>
-        <v>0.17498012629708</v>
+        <v>0.201583530316864</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))/H$40</f>
-        <v>0.274857878873534</v>
+        <v>0.208712080665388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
@@ -3988,27 +3988,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(C$15-$B35),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(C$15-$B36),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(C$15-$B37),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(C$15-$B38),$Q$43)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(C$15-$B39),$Q$43)))</f>
-        <v>4.05986344526568</v>
+        <v>4.99512612378856</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(D$15-$B35),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(D$15-$B36),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(D$15-$B37),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(D$15-$B38),$Q$43)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(D$15-$B39),$Q$43)))</f>
-        <v>4.07619804029952</v>
+        <v>4.90220325492284</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(E$15-$B35),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(E$15-$B36),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(E$15-$B37),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(E$15-$B38),$Q$43)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(E$15-$B39),$Q$43)))</f>
-        <v>4.08385981828578</v>
+        <v>4.96955299997369</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(F$15-$B35),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(F$15-$B36),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(F$15-$B37),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(F$15-$B38),$Q$43)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(F$15-$B39),$Q$43)))</f>
-        <v>4.03424844119736</v>
+        <v>4.95076713182323</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(G$15-$B35),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(G$15-$B36),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(G$15-$B37),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(G$15-$B38),$Q$43)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(G$15-$B39),$Q$43)))</f>
-        <v>4.28850463981276</v>
+        <v>4.8955045598091</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$L$43*POWER(ABS(H$15-$B35),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$L$43*POWER(ABS(H$15-$B36),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$L$43*POWER(ABS(H$15-$B37),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$L$43*POWER(ABS(H$15-$B38),$Q$43)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$L$43*POWER(ABS(H$15-$B39),$Q$43)))</f>
-        <v>3.63824389571206</v>
+        <v>4.79128949705227</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -4023,27 +4023,27 @@
       </c>
       <c r="C41" s="29" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.00199418325908482</v>
+        <v>0.0105817227158695</v>
       </c>
       <c r="D41" s="29" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.0130933519080281</v>
+        <v>0.00337381031364202</v>
       </c>
       <c r="E41" s="29" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.000763714741915464</v>
+        <v>0.0117745887953788</v>
       </c>
       <c r="F41" s="29" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.00343534072861075</v>
+        <v>0.00138705884106457</v>
       </c>
       <c r="G41" s="29" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.000169509891420603</v>
+        <v>0.00934995891526341</v>
       </c>
       <c r="H41" s="29" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.0166863788664341</v>
+        <v>0.00039469450712204</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -4079,27 +4079,27 @@
       </c>
       <c r="C42" s="29" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.00872516953386366</v>
+        <v>0.0184512056596577</v>
       </c>
       <c r="D42" s="29" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0172594982665032</v>
+        <v>0.00609189412556589</v>
       </c>
       <c r="E42" s="29" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.000100273285061121</v>
+        <v>0.0189397873915732</v>
       </c>
       <c r="F42" s="29" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.0123086791764945</v>
+        <v>0.0182591881603003</v>
       </c>
       <c r="G42" s="29" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.0194610762968659</v>
+        <v>0.0110930049046874</v>
       </c>
       <c r="H42" s="29" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.00824648159556091</v>
+        <v>0.0094037720747292</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
@@ -4125,11 +4125,11 @@
       </c>
       <c r="Q42" s="29" t="n">
         <f aca="false">agent1!Q42</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="29" t="n">
         <f aca="false">agent1!R42</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
@@ -4141,27 +4141,27 @@
       </c>
       <c r="C43" s="29" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.013555175466463</v>
+        <v>0.0139881416969001</v>
       </c>
       <c r="D43" s="29" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.00714858678169549</v>
+        <v>0.00274107585661113</v>
       </c>
       <c r="E43" s="29" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.00551540325395763</v>
+        <v>0.0114915249776095</v>
       </c>
       <c r="F43" s="29" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.0180970652773976</v>
+        <v>0.00141905183903873</v>
       </c>
       <c r="G43" s="29" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0120156239625067</v>
+        <v>0.00722982559353113</v>
       </c>
       <c r="H43" s="29" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.0146372821927071</v>
+        <v>0.0126443698536605</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
@@ -4172,26 +4172,26 @@
       </c>
       <c r="L43" s="29" t="n">
         <f aca="false">agent1!L43</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="29" t="n">
         <f aca="false">agent1!M43</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O43" s="9" t="s">
         <v>45</v>
       </c>
       <c r="P43" s="29" t="n">
         <f aca="false">agent1!P43</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="Q43" s="29" t="n">
         <f aca="false">agent1!Q43</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="R43" s="29" t="n">
         <f aca="false">agent1!R43</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="44">
@@ -4201,27 +4201,27 @@
       </c>
       <c r="C44" s="29" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.0192281497269869</v>
+        <v>0.000739569533616304</v>
       </c>
       <c r="D44" s="29" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.0159817668329924</v>
+        <v>0.0150425574183464</v>
       </c>
       <c r="E44" s="29" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.0144657478109002</v>
+        <v>0.00463722894899547</v>
       </c>
       <c r="F44" s="29" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.0140572618227452</v>
+        <v>0.00403010819107294</v>
       </c>
       <c r="G44" s="29" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.00430205968208611</v>
+        <v>0.0132340937387198</v>
       </c>
       <c r="H44" s="29" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.00903766732662916</v>
+        <v>0.01753646873869</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
@@ -4232,26 +4232,26 @@
       </c>
       <c r="L44" s="29" t="n">
         <f aca="false">agent1!L44</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="29" t="n">
         <f aca="false">agent1!M44</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="P44" s="29" t="n">
         <f aca="false">agent1!P44</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="29" t="n">
         <f aca="false">agent1!Q44</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="R44" s="29" t="n">
         <f aca="false">agent1!R44</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="45">
@@ -4261,27 +4261,27 @@
       </c>
       <c r="C45" s="29" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.00735592100769281</v>
+        <v>0.0124988691601902</v>
       </c>
       <c r="D45" s="29" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.00809176839888096</v>
+        <v>0.0151757281553</v>
       </c>
       <c r="E45" s="29" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.00392105360515416</v>
+        <v>0.0135235544107854</v>
       </c>
       <c r="F45" s="29" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.0018128377571702</v>
+        <v>0.00767658988945186</v>
       </c>
       <c r="G45" s="29" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.0165006668120623</v>
+        <v>0.0133300308045</v>
       </c>
       <c r="H45" s="29" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.0048676382098347</v>
+        <v>0.0126045751944184</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -4295,27 +4295,27 @@
       </c>
       <c r="C46" s="29" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.00264850493520498</v>
+        <v>0.00602100984193385</v>
       </c>
       <c r="D46" s="29" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.0157288165483624</v>
+        <v>0.0140696003381163</v>
       </c>
       <c r="E46" s="29" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.000849405042827129</v>
+        <v>0.00764713262207806</v>
       </c>
       <c r="F46" s="29" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.0171142527554184</v>
+        <v>0.0106582388002425</v>
       </c>
       <c r="G46" s="29" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.00978607837110758</v>
+        <v>0.0180997085291892</v>
       </c>
       <c r="H46" s="29" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.00515146472491324</v>
+        <v>0.000881226360797882</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -4325,27 +4325,27 @@
       </c>
       <c r="C47" s="29" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.00615192008204758</v>
+        <v>0.00819470753893256</v>
       </c>
       <c r="D47" s="29" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.0117802616301924</v>
+        <v>0.00868143124505878</v>
       </c>
       <c r="E47" s="29" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.0182448166422546</v>
+        <v>0.00425503667443991</v>
       </c>
       <c r="F47" s="29" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.00691563482396305</v>
+        <v>0.0199692963436246</v>
       </c>
       <c r="G47" s="29" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.0152156023681164</v>
+        <v>0.0100684900954366</v>
       </c>
       <c r="H47" s="29" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.0184143265336752</v>
+        <v>0.0136049955897033</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -4355,27 +4355,27 @@
       </c>
       <c r="C48" s="29" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.00360201369971037</v>
+        <v>0.000363990850746632</v>
       </c>
       <c r="D48" s="29" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.00394077190198004</v>
+        <v>0.00851969575509429</v>
       </c>
       <c r="E48" s="29" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.0156738248001784</v>
+        <v>0.0196968897152692</v>
       </c>
       <c r="F48" s="29" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.00370228698477149</v>
+        <v>0.0193037782423198</v>
       </c>
       <c r="G48" s="29" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.0162494510784745</v>
+        <v>0.00677888391539454</v>
       </c>
       <c r="H48" s="29" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.0151349011063576</v>
+        <v>0.0107898946292698</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -4385,27 +4385,27 @@
       </c>
       <c r="C49" s="29" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.0119487685803324</v>
+        <v>0.00870755031704903</v>
       </c>
       <c r="D49" s="29" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.00980462655425072</v>
+        <v>0.000767025612294674</v>
       </c>
       <c r="E49" s="29" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.00228348788805306</v>
+        <v>0.013530970485881</v>
       </c>
       <c r="F49" s="29" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.01746417183429</v>
+        <v>0.000199075294658542</v>
       </c>
       <c r="G49" s="29" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.00790169183164835</v>
+        <v>0.00218607746064663</v>
       </c>
       <c r="H49" s="29" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.0142991118505597</v>
+        <v>0.000760796079412103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -4415,27 +4415,27 @@
       </c>
       <c r="C50" s="29" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.0121014540269971</v>
+        <v>0.012843445148319</v>
       </c>
       <c r="D50" s="29" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.0152576128486544</v>
+        <v>0.0146849466208369</v>
       </c>
       <c r="E50" s="29" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.00239088024944067</v>
+        <v>0.0159365242347121</v>
       </c>
       <c r="F50" s="29" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.0160225076321512</v>
+        <v>0.00636699956841767</v>
       </c>
       <c r="G50" s="29" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.0170704506058246</v>
+        <v>0.00236153651028872</v>
       </c>
       <c r="H50" s="29" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.0188915470615029</v>
+        <v>0.00926655503921211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
@@ -4715,12 +4715,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1137254901961"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.74901960784314"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -5861,27 +5861,27 @@
       </c>
       <c r="C35" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))/C$40</f>
-        <v>0.207915113468915</v>
+        <v>0.18163923201665</v>
       </c>
       <c r="D35" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))/D$40</f>
-        <v>0.188162639784319</v>
+        <v>0.191833839128142</v>
       </c>
       <c r="E35" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))/E$40</f>
-        <v>0.193447337411528</v>
+        <v>0.196741138085732</v>
       </c>
       <c r="F35" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))/F$40</f>
-        <v>0.160875333369661</v>
+        <v>0.181853834937568</v>
       </c>
       <c r="G35" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))/G$40</f>
-        <v>0.151050437541635</v>
+        <v>0.162084438960403</v>
       </c>
       <c r="H35" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))/H$40</f>
-        <v>0.145158143046964</v>
+        <v>0.195979951383269</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -5893,27 +5893,27 @@
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))/C$40</f>
-        <v>0.231112417866771</v>
+        <v>0.205427006550911</v>
       </c>
       <c r="D36" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))/D$40</f>
-        <v>0.23632860588477</v>
+        <v>0.20255410103744</v>
       </c>
       <c r="E36" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))/E$40</f>
-        <v>0.23506154549525</v>
+        <v>0.201045335002003</v>
       </c>
       <c r="F36" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))/F$40</f>
-        <v>0.18392238272885</v>
+        <v>0.191367385765826</v>
       </c>
       <c r="G36" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))/G$40</f>
-        <v>0.191167582011692</v>
+        <v>0.185896797861139</v>
       </c>
       <c r="H36" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))/H$40</f>
-        <v>0.170104722823743</v>
+        <v>0.198159951311282</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
@@ -5924,27 +5924,27 @@
       </c>
       <c r="C37" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))/C$40</f>
-        <v>0.210051970533556</v>
+        <v>0.225867522864878</v>
       </c>
       <c r="D37" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))/D$40</f>
-        <v>0.235996744893708</v>
+        <v>0.211224119668836</v>
       </c>
       <c r="E37" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))/E$40</f>
-        <v>0.228823094892995</v>
+        <v>0.20442705382453</v>
       </c>
       <c r="F37" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))/F$40</f>
-        <v>0.208803062107524</v>
+        <v>0.200706373548786</v>
       </c>
       <c r="G37" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))/G$40</f>
-        <v>0.235649888796073</v>
+        <v>0.21033656318796</v>
       </c>
       <c r="H37" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))/H$40</f>
-        <v>0.19806958607857</v>
+        <v>0.200218905576433</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="13"/>
@@ -5955,27 +5955,27 @@
       </c>
       <c r="C38" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))/C$40</f>
-        <v>0.186522067609348</v>
+        <v>0.205427006550911</v>
       </c>
       <c r="D38" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))/D$40</f>
-        <v>0.19073185513672</v>
+        <v>0.20255410103744</v>
       </c>
       <c r="E38" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))/E$40</f>
-        <v>0.189709258749124</v>
+        <v>0.201045335002003</v>
       </c>
       <c r="F38" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))/F$40</f>
-        <v>0.233381851369678</v>
+        <v>0.20951146383095</v>
       </c>
       <c r="G38" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))/G$40</f>
-        <v>0.23194800333608</v>
+        <v>0.231345636802538</v>
       </c>
       <c r="H38" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))/H$40</f>
-        <v>0.228504892833997</v>
+        <v>0.202092542054183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
@@ -5984,27 +5984,27 @@
       </c>
       <c r="C39" s="22" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))/C$40</f>
-        <v>0.16439843052141</v>
+        <v>0.18163923201665</v>
       </c>
       <c r="D39" s="22" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))/D$40</f>
-        <v>0.148780154300482</v>
+        <v>0.191833839128142</v>
       </c>
       <c r="E39" s="22" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))/E$40</f>
-        <v>0.152958763451102</v>
+        <v>0.196741138085732</v>
       </c>
       <c r="F39" s="22" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))/F$40</f>
-        <v>0.213017370424287</v>
+        <v>0.21656094191687</v>
       </c>
       <c r="G39" s="22" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))/G$40</f>
-        <v>0.190184088314521</v>
+        <v>0.21033656318796</v>
       </c>
       <c r="H39" s="22" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))/H$40</f>
-        <v>0.258162655216726</v>
+        <v>0.203548649674833</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
@@ -6016,27 +6016,27 @@
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(C$15-$B35),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(C$15-$B36),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(C$15-$B37),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(C$15-$B38),$R$44)))+EXP((-C$44*POWER(ABS(MIN(C$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(C$15-$B39),$R$44)))</f>
-        <v>4.3076835496357</v>
+        <v>4.4273740080739</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(D$15-$B35),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(D$15-$B36),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(D$15-$B37),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(D$15-$B38),$R$44)))+EXP((-D$44*POWER(ABS(MIN(D$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(D$15-$B39),$R$44)))</f>
-        <v>3.83410973928261</v>
+        <v>4.73430781280014</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(E$15-$B35),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(E$15-$B36),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(E$15-$B37),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(E$15-$B38),$R$44)))+EXP((-E$44*POWER(ABS(MIN(E$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(E$15-$B39),$R$44)))</f>
-        <v>3.95430984996987</v>
+        <v>4.89172045133688</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(F$15-$B35),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(F$15-$B36),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(F$15-$B37),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(F$15-$B38),$R$44)))+EXP((-F$44*POWER(ABS(MIN(F$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(F$15-$B39),$R$44)))</f>
-        <v>4.24771658871625</v>
+        <v>4.61763783971657</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(G$15-$B35),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(G$15-$B36),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(G$15-$B37),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(G$15-$B38),$R$44)))+EXP((-G$44*POWER(ABS(MIN(G$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(G$15-$B39),$R$44)))</f>
-        <v>3.90103559859016</v>
+        <v>4.32253667638235</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B35),$B$40))+(-$M$44*POWER(ABS(H$15-$B35),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B36),$B$40))+(-$M$44*POWER(ABS(H$15-$B36),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B37),$B$40))+(-$M$44*POWER(ABS(H$15-$B37),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B38),$B$40))+(-$M$44*POWER(ABS(H$15-$B38),$R$44)))+EXP((-H$44*POWER(ABS(MIN(H$15+1,4)-$B39),$B$40))+(-$M$44*POWER(ABS(H$15-$B39),$R$44)))</f>
-        <v>3.87352694044964</v>
+        <v>4.91283042946975</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>21</v>
@@ -6051,27 +6051,27 @@
       </c>
       <c r="C41" s="34" t="n">
         <f aca="true">agent1!C41+$A$43*RAND()</f>
-        <v>0.0344550781417638</v>
+        <v>0.0374996687285602</v>
       </c>
       <c r="D41" s="34" t="n">
         <f aca="true">agent1!D41+$A$43*RAND()</f>
-        <v>0.014925641939044</v>
+        <v>0.0361774635035545</v>
       </c>
       <c r="E41" s="34" t="n">
         <f aca="true">agent1!E41+$A$43*RAND()</f>
-        <v>0.0809335181023926</v>
+        <v>0.0505864758510143</v>
       </c>
       <c r="F41" s="34" t="n">
         <f aca="true">agent1!F41+$A$43*RAND()</f>
-        <v>0.0256791613530368</v>
+        <v>0.0587748521473259</v>
       </c>
       <c r="G41" s="34" t="n">
         <f aca="true">agent1!G41+$A$43*RAND()</f>
-        <v>0.0495038160588592</v>
+        <v>0.0360239452216774</v>
       </c>
       <c r="H41" s="34" t="n">
         <f aca="true">agent1!H41+$A$43*RAND()</f>
-        <v>0.0570115299429745</v>
+        <v>0.000928926328197122</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>37</v>
@@ -6107,27 +6107,27 @@
       </c>
       <c r="C42" s="34" t="n">
         <f aca="true">agent1!C42+$A$43*RAND()</f>
-        <v>0.0177507940214127</v>
+        <v>0.0267998300958425</v>
       </c>
       <c r="D42" s="34" t="n">
         <f aca="true">agent1!D42+$A$43*RAND()</f>
-        <v>0.0675138845574111</v>
+        <v>0.0378438994754106</v>
       </c>
       <c r="E42" s="34" t="n">
         <f aca="true">agent1!E42+$A$43*RAND()</f>
-        <v>0.0767153894528747</v>
+        <v>0.0435274051036686</v>
       </c>
       <c r="F42" s="34" t="n">
         <f aca="true">agent1!F42+$A$43*RAND()</f>
-        <v>0.0961199180223048</v>
+        <v>0.0252842787187546</v>
       </c>
       <c r="G42" s="34" t="n">
         <f aca="true">agent1!G42+$A$43*RAND()</f>
-        <v>0.0860253194812685</v>
+        <v>0.0343627906870097</v>
       </c>
       <c r="H42" s="34" t="n">
         <f aca="true">agent1!H42+$A$43*RAND()</f>
-        <v>0.0579626448452473</v>
+        <v>0.0774218246806413</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>43</v>
@@ -6153,11 +6153,11 @@
       </c>
       <c r="Q42" s="34" t="n">
         <f aca="false">agent1!Q42</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="R42" s="34" t="n">
         <f aca="false">agent1!R42</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
@@ -6169,27 +6169,27 @@
       </c>
       <c r="C43" s="34" t="n">
         <f aca="true">agent1!C43+$A$43*RAND()</f>
-        <v>0.0717944235540926</v>
+        <v>0.0792337518651038</v>
       </c>
       <c r="D43" s="34" t="n">
         <f aca="true">agent1!D43+$A$43*RAND()</f>
-        <v>0.0457691623829305</v>
+        <v>0.0779005422722548</v>
       </c>
       <c r="E43" s="34" t="n">
         <f aca="true">agent1!E43+$A$43*RAND()</f>
-        <v>0.00698577761650085</v>
+        <v>0.0812569527886808</v>
       </c>
       <c r="F43" s="34" t="n">
         <f aca="true">agent1!F43+$A$43*RAND()</f>
-        <v>0.083211862994358</v>
+        <v>0.0468886042945087</v>
       </c>
       <c r="G43" s="34" t="n">
         <f aca="true">agent1!G43+$A$43*RAND()</f>
-        <v>0.0330900215543807</v>
+        <v>0.0788959187455475</v>
       </c>
       <c r="H43" s="34" t="n">
         <f aca="true">agent1!H43+$A$43*RAND()</f>
-        <v>0.0464942368213087</v>
+        <v>0.0921873400919139</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>45</v>
@@ -6200,26 +6200,26 @@
       </c>
       <c r="L43" s="34" t="n">
         <f aca="false">agent1!L43</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="34" t="n">
         <f aca="false">agent1!M43</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O43" s="9" t="s">
         <v>45</v>
       </c>
       <c r="P43" s="34" t="n">
         <f aca="false">agent1!P43</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="Q43" s="34" t="n">
         <f aca="false">agent1!Q43</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="R43" s="34" t="n">
         <f aca="false">agent1!R43</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="44">
@@ -6229,27 +6229,27 @@
       </c>
       <c r="C44" s="34" t="n">
         <f aca="true">agent1!C44+$A$43*RAND()</f>
-        <v>0.00445072925649583</v>
+        <v>0.0948578738141805</v>
       </c>
       <c r="D44" s="34" t="n">
         <f aca="true">agent1!D44+$A$43*RAND()</f>
-        <v>0.098594777751714</v>
+        <v>0.0419127318076789</v>
       </c>
       <c r="E44" s="34" t="n">
         <f aca="true">agent1!E44+$A$43*RAND()</f>
-        <v>0.0731018180493265</v>
+        <v>0.0166807769332081</v>
       </c>
       <c r="F44" s="34" t="n">
         <f aca="true">agent1!F44+$A$43*RAND()</f>
-        <v>0.00869775447063148</v>
+        <v>0.0330935369245708</v>
       </c>
       <c r="G44" s="34" t="n">
         <f aca="true">agent1!G44+$A$43*RAND()</f>
-        <v>0.0841660415288061</v>
+        <v>0.0952039258088917</v>
       </c>
       <c r="H44" s="34" t="n">
         <f aca="true">agent1!H44+$A$43*RAND()</f>
-        <v>0.0220322099048644</v>
+        <v>0.00717931957915425</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>47</v>
@@ -6260,26 +6260,26 @@
       </c>
       <c r="L44" s="34" t="n">
         <f aca="false">agent1!L44</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="34" t="n">
         <f aca="false">agent1!M44</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="P44" s="34" t="n">
         <f aca="false">agent1!P44</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="34" t="n">
         <f aca="false">agent1!Q44</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="R44" s="34" t="n">
         <f aca="false">agent1!R44</f>
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="45">
@@ -6289,27 +6289,27 @@
       </c>
       <c r="C45" s="34" t="n">
         <f aca="true">agent1!C45+$A$43*RAND()</f>
-        <v>0.0547074222471565</v>
+        <v>0.0506925846915692</v>
       </c>
       <c r="D45" s="34" t="n">
         <f aca="true">agent1!D45+$A$43*RAND()</f>
-        <v>0.0935972916893661</v>
+        <v>0.0431131445337087</v>
       </c>
       <c r="E45" s="34" t="n">
         <f aca="true">agent1!E45+$A$43*RAND()</f>
-        <v>0.0227823010645807</v>
+        <v>0.0656120731960982</v>
       </c>
       <c r="F45" s="34" t="n">
         <f aca="true">agent1!F45+$A$43*RAND()</f>
-        <v>0.0666618234943599</v>
+        <v>0.0303752058651298</v>
       </c>
       <c r="G45" s="34" t="n">
         <f aca="true">agent1!G45+$A$43*RAND()</f>
-        <v>0.0737098298966885</v>
+        <v>0.074948142375797</v>
       </c>
       <c r="H45" s="34" t="n">
         <f aca="true">agent1!H45+$A$43*RAND()</f>
-        <v>0.00813455409370363</v>
+        <v>0.0774197557475418</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="16"/>
@@ -6323,27 +6323,27 @@
       </c>
       <c r="C46" s="34" t="n">
         <f aca="true">agent1!C46+$A$43*RAND()</f>
-        <v>0.0611195588484407</v>
+        <v>0.0767079811077565</v>
       </c>
       <c r="D46" s="34" t="n">
         <f aca="true">agent1!D46+$A$43*RAND()</f>
-        <v>0.0781605591531843</v>
+        <v>0.0698060161899775</v>
       </c>
       <c r="E46" s="34" t="n">
         <f aca="true">agent1!E46+$A$43*RAND()</f>
-        <v>0.00672933184541762</v>
+        <v>0.0193324875552207</v>
       </c>
       <c r="F46" s="34" t="n">
         <f aca="true">agent1!F46+$A$43*RAND()</f>
-        <v>0.0342213768977672</v>
+        <v>0.0933887580409646</v>
       </c>
       <c r="G46" s="34" t="n">
         <f aca="true">agent1!G46+$A$43*RAND()</f>
-        <v>0.0868583136238158</v>
+        <v>0.00289955316111445</v>
       </c>
       <c r="H46" s="34" t="n">
         <f aca="true">agent1!H46+$A$43*RAND()</f>
-        <v>0.0908953733742237</v>
+        <v>0.0145364133641124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
@@ -6353,27 +6353,27 @@
       </c>
       <c r="C47" s="34" t="n">
         <f aca="true">agent1!C47+$A$43*RAND()</f>
-        <v>0.0562535868491977</v>
+        <v>0.000568077620118856</v>
       </c>
       <c r="D47" s="34" t="n">
         <f aca="true">agent1!D47+$A$43*RAND()</f>
-        <v>0.0213133917655796</v>
+        <v>0.0403992218896747</v>
       </c>
       <c r="E47" s="34" t="n">
         <f aca="true">agent1!E47+$A$43*RAND()</f>
-        <v>0.00582101531326771</v>
+        <v>0.050713876914233</v>
       </c>
       <c r="F47" s="34" t="n">
         <f aca="true">agent1!F47+$A$43*RAND()</f>
-        <v>0.0371871049515903</v>
+        <v>0.0511545534711331</v>
       </c>
       <c r="G47" s="34" t="n">
         <f aca="true">agent1!G47+$A$43*RAND()</f>
-        <v>0.0469925531186163</v>
+        <v>0.0991740740370005</v>
       </c>
       <c r="H47" s="34" t="n">
         <f aca="true">agent1!H47+$A$43*RAND()</f>
-        <v>0.0553248314186931</v>
+        <v>0.0867378221359104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
@@ -6383,27 +6383,27 @@
       </c>
       <c r="C48" s="34" t="n">
         <f aca="true">agent1!C48+$A$43*RAND()</f>
-        <v>0.0941986348945648</v>
+        <v>0.0520834797993302</v>
       </c>
       <c r="D48" s="34" t="n">
         <f aca="true">agent1!D48+$A$43*RAND()</f>
-        <v>0.0647433471400291</v>
+        <v>0.0259739041794091</v>
       </c>
       <c r="E48" s="34" t="n">
         <f aca="true">agent1!E48+$A$43*RAND()</f>
-        <v>0.0228387159761041</v>
+        <v>0.0245817216578871</v>
       </c>
       <c r="F48" s="34" t="n">
         <f aca="true">agent1!F48+$A$43*RAND()</f>
-        <v>0.0709140243474394</v>
+        <v>0.0956108849029988</v>
       </c>
       <c r="G48" s="34" t="n">
         <f aca="true">agent1!G48+$A$43*RAND()</f>
-        <v>0.0608632652089</v>
+        <v>0.0512581828981638</v>
       </c>
       <c r="H48" s="34" t="n">
         <f aca="true">agent1!H48+$A$43*RAND()</f>
-        <v>0.00886403550393879</v>
+        <v>0.0589445123448968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
@@ -6413,27 +6413,27 @@
       </c>
       <c r="C49" s="34" t="n">
         <f aca="true">agent1!C49+$A$43*RAND()</f>
-        <v>0.0288766691926867</v>
+        <v>0.0730327096302062</v>
       </c>
       <c r="D49" s="34" t="n">
         <f aca="true">agent1!D49+$A$43*RAND()</f>
-        <v>0.0326576887629926</v>
+        <v>0.0304919347632676</v>
       </c>
       <c r="E49" s="34" t="n">
         <f aca="true">agent1!E49+$A$43*RAND()</f>
-        <v>0.0546331978868693</v>
+        <v>0.0368450546637177</v>
       </c>
       <c r="F49" s="34" t="n">
         <f aca="true">agent1!F49+$A$43*RAND()</f>
-        <v>0.0358624468557537</v>
+        <v>0.054289662418887</v>
       </c>
       <c r="G49" s="34" t="n">
         <f aca="true">agent1!G49+$A$43*RAND()</f>
-        <v>0.0158695518039167</v>
+        <v>0.0773805390577763</v>
       </c>
       <c r="H49" s="34" t="n">
         <f aca="true">agent1!H49+$A$43*RAND()</f>
-        <v>0.0877232194878161</v>
+        <v>0.0157409734092653</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
@@ -6443,27 +6443,27 @@
       </c>
       <c r="C50" s="34" t="n">
         <f aca="true">agent1!C50+$A$43*RAND()</f>
-        <v>0.0823566836770624</v>
+        <v>0.046477002510801</v>
       </c>
       <c r="D50" s="34" t="n">
         <f aca="true">agent1!D50+$A$43*RAND()</f>
-        <v>0.0705769740510732</v>
+        <v>0.0280731237493455</v>
       </c>
       <c r="E50" s="34" t="n">
         <f aca="true">agent1!E50+$A$43*RAND()</f>
-        <v>0.0813205111771822</v>
+        <v>0.058854117942974</v>
       </c>
       <c r="F50" s="34" t="n">
         <f aca="true">agent1!F50+$A$43*RAND()</f>
-        <v>0.00513898474164307</v>
+        <v>0.0120890757068992</v>
       </c>
       <c r="G50" s="34" t="n">
         <f aca="true">agent1!G50+$A$43*RAND()</f>
-        <v>0.0372387975919992</v>
+        <v>0.0584483296144754</v>
       </c>
       <c r="H50" s="34" t="n">
         <f aca="true">agent1!H50+$A$43*RAND()</f>
-        <v>0.0550303410738707</v>
+        <v>0.033802260318771</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">

</xml_diff>